<commit_message>
Grades 1st quiz/Lecture 4
</commit_message>
<xml_diff>
--- a/phy140/Grades/grades_report_2023.xlsx
+++ b/phy140/Grades/grades_report_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ptohos/Documents/MyCourses/FYS140/2023/Grades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40486F39-926D-544F-9FD9-97189D10BECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBF7D46-335D-1D4A-8037-87A2BC2EB2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9760" yWindow="1000" windowWidth="35840" windowHeight="21900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5880" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quizzes" sheetId="5" r:id="rId1"/>
@@ -160,9 +160,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -248,6 +248,12 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF92D050"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -343,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -373,13 +379,13 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -397,7 +403,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -415,10 +421,25 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -735,9 +756,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BCA0582-B44F-2E45-BD0F-3C600431256F}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -791,7 +812,9 @@
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="27">
+        <v>5</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -801,16 +824,18 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B2/$B$49+C2/$C$49+D2/$D$49+E2/$E$49+F2/$F$49+G2/$G$49+H2/$H$49+I2/$I$49+J2/$J$49+K2/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L2" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B2/$B$50+C2/$C$50+D2/$D$50+E2/$E$50+F2/$F$50+G2/$G$50+H2/$H$50+I2/$I$50+J2/$J$50+K2/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="27">
+        <v>7</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -820,16 +845,18 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B3/$B$49+C3/$C$49+D3/$D$49+E3/$E$49+F3/$F$49+G3/$G$49+H3/$H$49+I3/$I$49+J3/$J$49+K3/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L3" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B3/$B$50+C3/$C$50+D3/$D$50+E3/$E$50+F3/$F$50+G3/$G$50+H3/$H$50+I3/$I$50+J3/$J$50+K3/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.46666666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="28">
+        <v>11</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -839,16 +866,18 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B4/$B$49+C4/$C$49+D4/$D$49+E4/$E$49+F4/$F$49+G4/$G$49+H4/$H$49+I4/$I$49+J4/$J$49+K4/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L4" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B4/$B$50+C4/$C$50+D4/$D$50+E4/$E$50+F4/$F$50+G4/$G$50+H4/$H$50+I4/$I$50+J4/$J$50+K4/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.73333333333333328</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="28">
+        <v>2</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -858,16 +887,18 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B5/$B$49+C5/$C$49+D5/$D$49+E5/$E$49+F5/$F$49+G5/$G$49+H5/$H$49+I5/$I$49+J5/$J$49+K5/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L5" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B5/$B$50+C5/$C$50+D5/$D$50+E5/$E$50+F5/$F$50+G5/$G$50+H5/$H$50+I5/$I$50+J5/$J$50+K5/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.13333333333333333</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1670</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="28">
+        <v>11</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -877,16 +908,18 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B6/$B$49+C6/$C$49+D6/$D$49+E6/$E$49+F6/$F$49+G6/$G$49+H6/$H$49+I6/$I$49+J6/$J$49+K6/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L6" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B6/$B$50+C6/$C$50+D6/$D$50+E6/$E$50+F6/$F$50+G6/$G$50+H6/$H$50+I6/$I$50+J6/$J$50+K6/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.73333333333333328</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>1691</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="28">
+        <v>3</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -896,16 +929,18 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B7/$B$49+C7/$C$49+D7/$D$49+E7/$E$49+F7/$F$49+G7/$G$49+H7/$H$49+I7/$I$49+J7/$J$49+K7/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L7" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B7/$B$50+C7/$C$50+D7/$D$50+E7/$E$50+F7/$F$50+G7/$G$50+H7/$H$50+I7/$I$50+J7/$J$50+K7/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1889</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="28">
+        <v>2</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -915,16 +950,18 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B8/$B$49+C8/$C$49+D8/$D$49+E8/$E$49+F8/$F$49+G8/$G$49+H8/$H$49+I8/$I$49+J8/$J$49+K8/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L8" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B8/$B$50+C8/$C$50+D8/$D$50+E8/$E$50+F8/$F$50+G8/$G$50+H8/$H$50+I8/$I$50+J8/$J$50+K8/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.13333333333333333</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2085</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="28">
+        <v>3</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -934,16 +971,18 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B9/$B$49+C9/$C$49+D9/$D$49+E9/$E$49+F9/$F$49+G9/$G$49+H9/$H$49+I9/$I$49+J9/$J$49+K9/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L9" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B9/$B$50+C9/$C$50+D9/$D$50+E9/$E$50+F9/$F$50+G9/$G$50+H9/$H$50+I9/$I$50+J9/$J$50+K9/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2163</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="28">
+        <v>4</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -953,16 +992,18 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B10/$B$49+C10/$C$49+D10/$D$49+E10/$E$49+F10/$F$49+G10/$G$49+H10/$H$49+I10/$I$49+J10/$J$49+K10/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L10" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B10/$B$50+C10/$C$50+D10/$D$50+E10/$E$50+F10/$F$50+G10/$G$50+H10/$H$50+I10/$I$50+J10/$J$50+K10/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.26666666666666666</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2393</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="28">
+        <v>8</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -972,16 +1013,18 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B11/$B$49+C11/$C$49+D11/$D$49+E11/$E$49+F11/$F$49+G11/$G$49+H11/$H$49+I11/$I$49+J11/$J$49+K11/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L11" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B11/$B$50+C11/$C$50+D11/$D$50+E11/$E$50+F11/$F$50+G11/$G$50+H11/$H$50+I11/$I$50+J11/$J$50+K11/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.53333333333333333</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>2441</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="28">
+        <v>10</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -991,16 +1034,18 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B12/$B$49+C12/$C$49+D12/$D$49+E12/$E$49+F12/$F$49+G12/$G$49+H12/$H$49+I12/$I$49+J12/$J$49+K12/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L12" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B12/$B$50+C12/$C$50+D12/$D$50+E12/$E$50+F12/$F$50+G12/$G$50+H12/$H$50+I12/$I$50+J12/$J$50+K12/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>2903</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="28">
+        <v>3</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1010,16 +1055,18 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B13/$B$49+C13/$C$49+D13/$D$49+E13/$E$49+F13/$F$49+G13/$G$49+H13/$H$49+I13/$I$49+J13/$J$49+K13/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L13" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B13/$B$50+C13/$C$50+D13/$D$50+E13/$E$50+F13/$F$50+G13/$G$50+H13/$H$50+I13/$I$50+J13/$J$50+K13/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>2994</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="28">
+        <v>7</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1029,16 +1076,18 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B14/$B$49+C14/$C$49+D14/$D$49+E14/$E$49+F14/$F$49+G14/$G$49+H14/$H$49+I14/$I$49+J14/$J$49+K14/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L14" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B14/$B$50+C14/$C$50+D14/$D$50+E14/$E$50+F14/$F$50+G14/$G$50+H14/$H$50+I14/$I$50+J14/$J$50+K14/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.46666666666666667</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>3377</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="28">
+        <v>6</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1048,16 +1097,18 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B15/$B$49+C15/$C$49+D15/$D$49+E15/$E$49+F15/$F$49+G15/$G$49+H15/$H$49+I15/$I$49+J15/$J$49+K15/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L15" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B15/$B$50+C15/$C$50+D15/$D$50+E15/$E$50+F15/$F$50+G15/$G$50+H15/$H$50+I15/$I$50+J15/$J$50+K15/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>3517</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="28">
+        <v>8</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1067,16 +1118,18 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B16/$B$49+C16/$C$49+D16/$D$49+E16/$E$49+F16/$F$49+G16/$G$49+H16/$H$49+I16/$I$49+J16/$J$49+K16/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L16" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B16/$B$50+C16/$C$50+D16/$D$50+E16/$E$50+F16/$F$50+G16/$G$50+H16/$H$50+I16/$I$50+J16/$J$50+K16/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.53333333333333333</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>3560</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="28">
+        <v>7</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -1086,16 +1139,16 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B17/$B$49+C17/$C$49+D17/$D$49+E17/$E$49+F17/$F$49+G17/$G$49+H17/$H$49+I17/$I$49+J17/$J$49+K17/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L17" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B17/$B$50+C17/$C$50+D17/$D$50+E17/$E$50+F17/$F$50+G17/$G$50+H17/$H$50+I17/$I$50+J17/$J$50+K17/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.46666666666666667</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>3601</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1105,8 +1158,8 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B18/$B$49+C18/$C$49+D18/$D$49+E18/$E$49+F18/$F$49+G18/$G$49+H18/$H$49+I18/$I$49+J18/$J$49+K18/$K$49)/SUM(B$53:$K$53),0)</f>
+      <c r="L18" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B18/$B$50+C18/$C$50+D18/$D$50+E18/$E$50+F18/$F$50+G18/$G$50+H18/$H$50+I18/$I$50+J18/$J$50+K18/$K$50)/SUM(B$54:$K$54),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1114,7 +1167,9 @@
       <c r="A19" s="2">
         <v>3642</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="28">
+        <v>5</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1124,16 +1179,18 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B19/$B$49+C19/$C$49+D19/$D$49+E19/$E$49+F19/$F$49+G19/$G$49+H19/$H$49+I19/$I$49+J19/$J$49+K19/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L19" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B19/$B$50+C19/$C$50+D19/$D$50+E19/$E$50+F19/$F$50+G19/$G$50+H19/$H$50+I19/$I$50+J19/$J$50+K19/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>3672</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="28">
+        <v>12</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1143,16 +1200,18 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-      <c r="L20" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B20/$B$49+C20/$C$49+D20/$D$49+E20/$E$49+F20/$F$49+G20/$G$49+H20/$H$49+I20/$I$49+J20/$J$49+K20/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L20" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B20/$B$50+C20/$C$50+D20/$D$50+E20/$E$50+F20/$F$50+G20/$G$50+H20/$H$50+I20/$I$50+J20/$J$50+K20/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.8</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>3797</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="28">
+        <v>10</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1162,16 +1221,18 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B21/$B$49+C21/$C$49+D21/$D$49+E21/$E$49+F21/$F$49+G21/$G$49+H21/$H$49+I21/$I$49+J21/$J$49+K21/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L21" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B21/$B$50+C21/$C$50+D21/$D$50+E21/$E$50+F21/$F$50+G21/$G$50+H21/$H$50+I21/$I$50+J21/$J$50+K21/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>4091</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="28">
+        <v>10</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1181,16 +1242,16 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B22/$B$49+C22/$C$49+D22/$D$49+E22/$E$49+F22/$F$49+G22/$G$49+H22/$H$49+I22/$I$49+J22/$J$49+K22/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L22" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B22/$B$50+C22/$C$50+D22/$D$50+E22/$E$50+F22/$F$50+G22/$G$50+H22/$H$50+I22/$I$50+J22/$J$50+K22/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>4582</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1200,8 +1261,8 @@
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B23/$B$49+C23/$C$49+D23/$D$49+E23/$E$49+F23/$F$49+G23/$G$49+H23/$H$49+I23/$I$49+J23/$J$49+K23/$K$49)/SUM(B$53:$K$53),0)</f>
+      <c r="L23" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B23/$B$50+C23/$C$50+D23/$D$50+E23/$E$50+F23/$F$50+G23/$G$50+H23/$H$50+I23/$I$50+J23/$J$50+K23/$K$50)/SUM(B$54:$K$54),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1209,7 +1270,9 @@
       <c r="A24" s="2">
         <v>4622</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="28">
+        <v>4</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1219,16 +1282,18 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-      <c r="L24" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B24/$B$49+C24/$C$49+D24/$D$49+E24/$E$49+F24/$F$49+G24/$G$49+H24/$H$49+I24/$I$49+J24/$J$49+K24/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L24" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B24/$B$50+C24/$C$50+D24/$D$50+E24/$E$50+F24/$F$50+G24/$G$50+H24/$H$50+I24/$I$50+J24/$J$50+K24/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.26666666666666666</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>5075</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="28">
+        <v>9</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1238,16 +1303,18 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
-      <c r="L25" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B25/$B$49+C25/$C$49+D25/$D$49+E25/$E$49+F25/$F$49+G25/$G$49+H25/$H$49+I25/$I$49+J25/$J$49+K25/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L25" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B25/$B$50+C25/$C$50+D25/$D$50+E25/$E$50+F25/$F$50+G25/$G$50+H25/$H$50+I25/$I$50+J25/$J$50+K25/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.6</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>5141</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="28">
+        <v>7</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1257,16 +1324,18 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="L26" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B26/$B$49+C26/$C$49+D26/$D$49+E26/$E$49+F26/$F$49+G26/$G$49+H26/$H$49+I26/$I$49+J26/$J$49+K26/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L26" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B26/$B$50+C26/$C$50+D26/$D$50+E26/$E$50+F26/$F$50+G26/$G$50+H26/$H$50+I26/$I$50+J26/$J$50+K26/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.46666666666666667</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>5482</v>
       </c>
-      <c r="B27" s="2"/>
+      <c r="B27" s="28">
+        <v>3</v>
+      </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1276,16 +1345,18 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
-      <c r="L27" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B27/$B$49+C27/$C$49+D27/$D$49+E27/$E$49+F27/$F$49+G27/$G$49+H27/$H$49+I27/$I$49+J27/$J$49+K27/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L27" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B27/$B$50+C27/$C$50+D27/$D$50+E27/$E$50+F27/$F$50+G27/$G$50+H27/$H$50+I27/$I$50+J27/$J$50+K27/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>5680</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="28">
+        <v>2</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1295,16 +1366,18 @@
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
-      <c r="L28" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B28/$B$49+C28/$C$49+D28/$D$49+E28/$E$49+F28/$F$49+G28/$G$49+H28/$H$49+I28/$I$49+J28/$J$49+K28/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L28" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B28/$B$50+C28/$C$50+D28/$D$50+E28/$E$50+F28/$F$50+G28/$G$50+H28/$H$50+I28/$I$50+J28/$J$50+K28/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.13333333333333333</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>5943</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="28">
+        <v>5</v>
+      </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1314,16 +1387,18 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B29/$B$49+C29/$C$49+D29/$D$49+E29/$E$49+F29/$F$49+G29/$G$49+H29/$H$49+I29/$I$49+J29/$J$49+K29/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L29" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B29/$B$50+C29/$C$50+D29/$D$50+E29/$E$50+F29/$F$50+G29/$G$50+H29/$H$50+I29/$I$50+J29/$J$50+K29/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>6464</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="28">
+        <v>10</v>
+      </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1333,16 +1408,18 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-      <c r="L30" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B30/$B$49+C30/$C$49+D30/$D$49+E30/$E$49+F30/$F$49+G30/$G$49+H30/$H$49+I30/$I$49+J30/$J$49+K30/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L30" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B30/$B$50+C30/$C$50+D30/$D$50+E30/$E$50+F30/$F$50+G30/$G$50+H30/$H$50+I30/$I$50+J30/$J$50+K30/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>6797</v>
       </c>
-      <c r="B31" s="2"/>
+      <c r="B31" s="28">
+        <v>5</v>
+      </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1352,16 +1429,18 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B31/$B$49+C31/$C$49+D31/$D$49+E31/$E$49+F31/$F$49+G31/$G$49+H31/$H$49+I31/$I$49+J31/$J$49+K31/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L31" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B31/$B$50+C31/$C$50+D31/$D$50+E31/$E$50+F31/$F$50+G31/$G$50+H31/$H$50+I31/$I$50+J31/$J$50+K31/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>7021</v>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B32" s="28">
+        <v>6</v>
+      </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1371,16 +1450,16 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B32/$B$49+C32/$C$49+D32/$D$49+E32/$E$49+F32/$F$49+G32/$G$49+H32/$H$49+I32/$I$49+J32/$J$49+K32/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L32" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B32/$B$50+C32/$C$50+D32/$D$50+E32/$E$50+F32/$F$50+G32/$G$50+H32/$H$50+I32/$I$50+J32/$J$50+K32/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.4</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>7575</v>
-      </c>
-      <c r="B33" s="2"/>
+        <v>7511</v>
+      </c>
+      <c r="B33" s="28"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1390,16 +1469,18 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
-      <c r="L33" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B33/$B$49+C33/$C$49+D33/$D$49+E33/$E$49+F33/$F$49+G33/$G$49+H33/$H$49+I33/$I$49+J33/$J$49+K33/$K$49)/SUM(B$53:$K$53),0)</f>
+      <c r="L33" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B33/$B$50+C33/$C$50+D33/$D$50+E33/$E$50+F33/$F$50+G33/$G$50+H33/$H$50+I33/$I$50+J33/$J$50+K33/$K$50)/SUM(B$54:$K$54),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>7642</v>
-      </c>
-      <c r="B34" s="2"/>
+        <v>7575</v>
+      </c>
+      <c r="B34" s="28">
+        <v>3</v>
+      </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1409,16 +1490,18 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
-      <c r="L34" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B34/$B$49+C34/$C$49+D34/$D$49+E34/$E$49+F34/$F$49+G34/$G$49+H34/$H$49+I34/$I$49+J34/$J$49+K34/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L34" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B34/$B$50+C34/$C$50+D34/$D$50+E34/$E$50+F34/$F$50+G34/$G$50+H34/$H$50+I34/$I$50+J34/$J$50+K34/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>7949</v>
-      </c>
-      <c r="B35" s="2"/>
+        <v>7642</v>
+      </c>
+      <c r="B35" s="28">
+        <v>3</v>
+      </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1428,16 +1511,16 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
-      <c r="L35" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B35/$B$49+C35/$C$49+D35/$D$49+E35/$E$49+F35/$F$49+G35/$G$49+H35/$H$49+I35/$I$49+J35/$J$49+K35/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L35" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B35/$B$50+C35/$C$50+D35/$D$50+E35/$E$50+F35/$F$50+G35/$G$50+H35/$H$50+I35/$I$50+J35/$J$50+K35/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>8688</v>
-      </c>
-      <c r="B36" s="2"/>
+        <v>7949</v>
+      </c>
+      <c r="B36" s="28"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1447,16 +1530,16 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
-      <c r="L36" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B36/$B$49+C36/$C$49+D36/$D$49+E36/$E$49+F36/$F$49+G36/$G$49+H36/$H$49+I36/$I$49+J36/$J$49+K36/$K$49)/SUM(B$53:$K$53),0)</f>
+      <c r="L36" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B36/$B$50+C36/$C$50+D36/$D$50+E36/$E$50+F36/$F$50+G36/$G$50+H36/$H$50+I36/$I$50+J36/$J$50+K36/$K$50)/SUM(B$54:$K$54),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>8742</v>
-      </c>
-      <c r="B37" s="2"/>
+        <v>8688</v>
+      </c>
+      <c r="B37" s="28"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1466,16 +1549,18 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="L37" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B37/$B$49+C37/$C$49+D37/$D$49+E37/$E$49+F37/$F$49+G37/$G$49+H37/$H$49+I37/$I$49+J37/$J$49+K37/$K$49)/SUM(B$53:$K$53),0)</f>
+      <c r="L37" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B37/$B$50+C37/$C$50+D37/$D$50+E37/$E$50+F37/$F$50+G37/$G$50+H37/$H$50+I37/$I$50+J37/$J$50+K37/$K$50)/SUM(B$54:$K$54),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>8743</v>
-      </c>
-      <c r="B38" s="2"/>
+        <v>8742</v>
+      </c>
+      <c r="B38" s="28">
+        <v>5</v>
+      </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1485,16 +1570,18 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
-      <c r="L38" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B38/$B$49+C38/$C$49+D38/$D$49+E38/$E$49+F38/$F$49+G38/$G$49+H38/$H$49+I38/$I$49+J38/$J$49+K38/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L38" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B38/$B$50+C38/$C$50+D38/$D$50+E38/$E$50+F38/$F$50+G38/$G$50+H38/$H$50+I38/$I$50+J38/$J$50+K38/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>8765</v>
-      </c>
-      <c r="B39" s="2"/>
+        <v>8743</v>
+      </c>
+      <c r="B39" s="28">
+        <v>6</v>
+      </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -1504,16 +1591,18 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
-      <c r="L39" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B39/$B$49+C39/$C$49+D39/$D$49+E39/$E$49+F39/$F$49+G39/$G$49+H39/$H$49+I39/$I$49+J39/$J$49+K39/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L39" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B39/$B$50+C39/$C$50+D39/$D$50+E39/$E$50+F39/$F$50+G39/$G$50+H39/$H$50+I39/$I$50+J39/$J$50+K39/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.4</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>8793</v>
-      </c>
-      <c r="B40" s="2"/>
+        <v>8765</v>
+      </c>
+      <c r="B40" s="28">
+        <v>6</v>
+      </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1523,16 +1612,18 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
-      <c r="L40" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B40/$B$49+C40/$C$49+D40/$D$49+E40/$E$49+F40/$F$49+G40/$G$49+H40/$H$49+I40/$I$49+J40/$J$49+K40/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L40" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B40/$B$50+C40/$C$50+D40/$D$50+E40/$E$50+F40/$F$50+G40/$G$50+H40/$H$50+I40/$I$50+J40/$J$50+K40/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.4</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>9139</v>
-      </c>
-      <c r="B41" s="2"/>
+        <v>8793</v>
+      </c>
+      <c r="B41" s="28">
+        <v>8</v>
+      </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1542,16 +1633,18 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
-      <c r="L41" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B41/$B$49+C41/$C$49+D41/$D$49+E41/$E$49+F41/$F$49+G41/$G$49+H41/$H$49+I41/$I$49+J41/$J$49+K41/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L41" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B41/$B$50+C41/$C$50+D41/$D$50+E41/$E$50+F41/$F$50+G41/$G$50+H41/$H$50+I41/$I$50+J41/$J$50+K41/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.53333333333333333</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>9196</v>
-      </c>
-      <c r="B42" s="2"/>
+        <v>9139</v>
+      </c>
+      <c r="B42" s="28">
+        <v>2</v>
+      </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1561,16 +1654,18 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-      <c r="L42" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B42/$B$49+C42/$C$49+D42/$D$49+E42/$E$49+F42/$F$49+G42/$G$49+H42/$H$49+I42/$I$49+J42/$J$49+K42/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L42" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B42/$B$50+C42/$C$50+D42/$D$50+E42/$E$50+F42/$F$50+G42/$G$50+H42/$H$50+I42/$I$50+J42/$J$50+K42/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.13333333333333333</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>9355</v>
-      </c>
-      <c r="B43" s="2"/>
+        <v>9196</v>
+      </c>
+      <c r="B43" s="28">
+        <v>7</v>
+      </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1580,16 +1675,18 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="L43" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B43/$B$49+C43/$C$49+D43/$D$49+E43/$E$49+F43/$F$49+G43/$G$49+H43/$H$49+I43/$I$49+J43/$J$49+K43/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L43" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B43/$B$50+C43/$C$50+D43/$D$50+E43/$E$50+F43/$F$50+G43/$G$50+H43/$H$50+I43/$I$50+J43/$J$50+K43/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.46666666666666667</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>9516</v>
-      </c>
-      <c r="B44" s="2"/>
+        <v>9355</v>
+      </c>
+      <c r="B44" s="28">
+        <v>8</v>
+      </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1599,16 +1696,16 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
-      <c r="L44" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B44/$B$49+C44/$C$49+D44/$D$49+E44/$E$49+F44/$F$49+G44/$G$49+H44/$H$49+I44/$I$49+J44/$J$49+K44/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L44" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B44/$B$50+C44/$C$50+D44/$D$50+E44/$E$50+F44/$F$50+G44/$G$50+H44/$H$50+I44/$I$50+J44/$J$50+K44/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.53333333333333333</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>9550</v>
-      </c>
-      <c r="B45" s="2"/>
+        <v>9516</v>
+      </c>
+      <c r="B45" s="28"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1618,16 +1715,18 @@
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
-      <c r="L45" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B45/$B$49+C45/$C$49+D45/$D$49+E45/$E$49+F45/$F$49+G45/$G$49+H45/$H$49+I45/$I$49+J45/$J$49+K45/$K$49)/SUM(B$53:$K$53),0)</f>
+      <c r="L45" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B45/$B$50+C45/$C$50+D45/$D$50+E45/$E$50+F45/$F$50+G45/$G$50+H45/$H$50+I45/$I$50+J45/$J$50+K45/$K$50)/SUM(B$54:$K$54),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>9744</v>
-      </c>
-      <c r="B46" s="2"/>
+        <v>9550</v>
+      </c>
+      <c r="B46" s="28">
+        <v>10</v>
+      </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1637,16 +1736,18 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-      <c r="L46" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B46/$B$49+C46/$C$49+D46/$D$49+E46/$E$49+F46/$F$49+G46/$G$49+H46/$H$49+I46/$I$49+J46/$J$49+K46/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
+      <c r="L46" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B46/$B$50+C46/$C$50+D46/$D$50+E46/$E$50+F46/$F$50+G46/$G$50+H46/$H$50+I46/$I$50+J46/$J$50+K46/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>9881</v>
-      </c>
-      <c r="B47" s="2"/>
+        <v>9744</v>
+      </c>
+      <c r="B47" s="28">
+        <v>5</v>
+      </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1656,242 +1757,263 @@
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-      <c r="L47" s="2">
-        <f>IF(SUM($B$53:$K$53)&gt;0,$L$49*(B47/$B$49+C47/$C$49+D47/$D$49+E47/$E$49+F47/$F$49+G47/$G$49+H47/$H$49+I47/$I$49+J47/$J$49+K47/$K$49)/SUM(B$53:$K$53),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+      <c r="L47" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B47/$B$50+C47/$C$50+D47/$D$50+E47/$E$50+F47/$F$50+G47/$G$50+H47/$H$50+I47/$I$50+J47/$J$50+K47/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>9881</v>
+      </c>
+      <c r="B48" s="28">
+        <v>7</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="29">
+        <f>IF(SUM($B$54:$K$54)&gt;0,$L$50*(B48/$B$50+C48/$C$50+D48/$D$50+E48/$E$50+F48/$F$50+G48/$G$50+H48/$H$50+I48/$I$50+J48/$J$50+K48/$K$50)/SUM(B$54:$K$54),0)</f>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="9">
-        <v>20</v>
-      </c>
-      <c r="C49" s="10">
+      <c r="B50" s="9">
         <v>15</v>
       </c>
-      <c r="D49" s="10">
+      <c r="C50" s="10">
         <v>15</v>
       </c>
-      <c r="E49" s="10">
+      <c r="D50" s="10">
         <v>15</v>
       </c>
-      <c r="F49" s="10">
+      <c r="E50" s="10">
         <v>15</v>
       </c>
-      <c r="G49" s="10">
+      <c r="F50" s="10">
         <v>15</v>
       </c>
-      <c r="H49" s="10">
+      <c r="G50" s="10">
         <v>15</v>
       </c>
-      <c r="I49" s="10">
+      <c r="H50" s="10">
         <v>15</v>
       </c>
-      <c r="J49" s="10">
+      <c r="I50" s="10">
         <v>15</v>
       </c>
-      <c r="K49" s="10">
+      <c r="J50" s="10">
         <v>15</v>
       </c>
-      <c r="L49" s="11">
+      <c r="K50" s="10">
+        <v>15</v>
+      </c>
+      <c r="L50" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="12" t="s">
+    <row r="51" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="13" t="e">
-        <f>AVERAGE(B$2:B$47)</f>
+      <c r="B51" s="13">
+        <f>AVERAGE(B$2:B$48)</f>
+        <v>6.2195121951219514</v>
+      </c>
+      <c r="C51" s="13" t="e">
+        <f t="shared" ref="C51:L51" si="0">AVERAGE(C$2:C$48)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C50" s="13" t="e">
-        <f t="shared" ref="C50:L50" si="0">AVERAGE(C$2:C$47)</f>
+      <c r="D51" s="13" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D50" s="13" t="e">
+      <c r="E51" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E50" s="13" t="e">
+      <c r="F51" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F50" s="13" t="e">
+      <c r="G51" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G50" s="13" t="e">
+      <c r="H51" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H50" s="13" t="e">
+      <c r="I51" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I50" s="13" t="e">
+      <c r="J51" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J50" s="13" t="e">
+      <c r="K51" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K50" s="13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L50" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" s="13" t="e">
-        <f>STDEV(B$2:B$47)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C51" s="13" t="e">
-        <f t="shared" ref="C51:L51" si="1">STDEV(C$2:C$47)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D51" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E51" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F51" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G51" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H51" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I51" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J51" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K51" s="13" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="L51" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.36170212765957438</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="13">
+        <f>STDEV(B$2:B$48)</f>
+        <v>2.8593023198146712</v>
+      </c>
+      <c r="C52" s="13" t="e">
+        <f t="shared" ref="C52:L52" si="1">STDEV(C$2:C$48)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D52" s="13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E52" s="13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F52" s="13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G52" s="13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H52" s="13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I52" s="13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J52" s="13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K52" s="13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L52" s="13">
+        <f t="shared" si="1"/>
+        <v>0.22618221069524505</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="13" t="e">
-        <f>MEDIAN(B$2:B$47)</f>
+      <c r="B53" s="13">
+        <f>MEDIAN(B$2:B$48)</f>
+        <v>6</v>
+      </c>
+      <c r="C53" s="13" t="e">
+        <f t="shared" ref="C53:L53" si="2">MEDIAN(C$2:C$48)</f>
         <v>#NUM!</v>
       </c>
-      <c r="C52" s="13" t="e">
-        <f t="shared" ref="C52:L52" si="2">MEDIAN(C$2:C$47)</f>
+      <c r="D53" s="13" t="e">
+        <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="D52" s="13" t="e">
+      <c r="E53" s="13" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="E52" s="13" t="e">
+      <c r="F53" s="13" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="F52" s="13" t="e">
+      <c r="G53" s="13" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="G52" s="13" t="e">
+      <c r="H53" s="13" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="H52" s="13" t="e">
+      <c r="I53" s="13" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="I52" s="13" t="e">
+      <c r="J53" s="13" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="J52" s="13" t="e">
+      <c r="K53" s="13" t="e">
         <f t="shared" si="2"/>
         <v>#NUM!</v>
       </c>
-      <c r="K52" s="13" t="e">
-        <f t="shared" si="2"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="L52" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="15" t="s">
+      <c r="L53" s="13">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B53" s="16">
-        <f t="shared" ref="B53:K53" si="3">IF(SUM(B11:B47)&gt;0,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C53" s="16">
+      <c r="B54" s="16">
+        <f t="shared" ref="B54:K54" si="3">IF(SUM(B11:B48)&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C54" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D53" s="16">
+      <c r="D54" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E53" s="16">
+      <c r="E54" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F53" s="16">
+      <c r="F54" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G53" s="16">
+      <c r="G54" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H53" s="16">
+      <c r="H54" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I53" s="16">
+      <c r="I54" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J53" s="16">
+      <c r="J54" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K53" s="16">
+      <c r="K54" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L53" s="10"/>
+      <c r="L54" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1903,10 +2025,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B60FCCA-9573-8140-9A4F-53646890C136}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J1048576"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1960,8 +2082,8 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2">
-        <f>IF(SUM($B$53:$I$53)&gt;0,$J$49*(B2/$B$49+C2/$C$49+D2/$D$49+E2/$E$49+F2/$F$49+G2/$G$49+H2/$H$49+I2/$I$49)/SUM($B$53:$I$53),0)</f>
+      <c r="J2" s="29">
+        <f t="shared" ref="J2:J48" si="0">IF(SUM($B$54:$I$54)&gt;0,$J$50*(B2/$B$50+C2/$C$50+D2/$D$50+E2/$E$50+F2/$F$50+G2/$G$50+H2/$H$50+I2/$I$50)/SUM($B$54:$I$54),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -1977,8 +2099,8 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="2">
-        <f t="shared" ref="J3:J47" si="0">IF(SUM($B$53:$I$53)&gt;0,$J$49*(B3/$B$49+C3/$C$49+D3/$D$49+E3/$E$49+F3/$F$49+G3/$G$49+H3/$H$49+I3/$I$49)/SUM($B$53:$I$53),0)</f>
+      <c r="J3" s="29">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1994,7 +2116,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2">
+      <c r="J4" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2011,7 +2133,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="2">
+      <c r="J5" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2028,7 +2150,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2">
+      <c r="J6" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2045,7 +2167,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="2">
+      <c r="J7" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2062,7 +2184,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2">
+      <c r="J8" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2079,7 +2201,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2">
+      <c r="J9" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2096,7 +2218,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2">
+      <c r="J10" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2113,7 +2235,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="2">
+      <c r="J11" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2130,7 +2252,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2">
+      <c r="J12" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2147,7 +2269,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="2">
+      <c r="J13" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2164,7 +2286,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2">
+      <c r="J14" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2181,7 +2303,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="2">
+      <c r="J15" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2198,7 +2320,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="2">
+      <c r="J16" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2215,7 +2337,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="J17" s="2">
+      <c r="J17" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2232,7 +2354,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="2">
+      <c r="J18" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2249,7 +2371,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="2">
+      <c r="J19" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2266,7 +2388,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="2">
+      <c r="J20" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2283,7 +2405,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="2">
+      <c r="J21" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2300,7 +2422,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2">
+      <c r="J22" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2317,7 +2439,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="2">
+      <c r="J23" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2334,7 +2456,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="2">
+      <c r="J24" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2351,7 +2473,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2">
+      <c r="J25" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2368,7 +2490,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-      <c r="J26" s="2">
+      <c r="J26" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2385,7 +2507,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="J27" s="2">
+      <c r="J27" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2402,7 +2524,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="J28" s="2">
+      <c r="J28" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2419,7 +2541,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="2">
+      <c r="J29" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2436,7 +2558,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="2">
+      <c r="J30" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2453,7 +2575,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="2">
+      <c r="J31" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2470,14 +2592,14 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="2">
+      <c r="J32" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>7575</v>
+        <v>7511</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2487,14 +2609,14 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="2">
+      <c r="J33" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>7642</v>
+        <v>7575</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2504,14 +2626,14 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="2">
+      <c r="J34" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>7949</v>
+        <v>7642</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2521,14 +2643,14 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="2">
+      <c r="J35" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>8688</v>
+        <v>7949</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2538,14 +2660,14 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="2">
+      <c r="J36" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>8742</v>
+        <v>8688</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2555,14 +2677,14 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="2">
+      <c r="J37" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>8743</v>
+        <v>8742</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2572,14 +2694,14 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
-      <c r="J38" s="2">
+      <c r="J38" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>8765</v>
+        <v>8743</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2589,14 +2711,14 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-      <c r="J39" s="2">
+      <c r="J39" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>8793</v>
+        <v>8765</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2606,14 +2728,14 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="2">
+      <c r="J40" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>9139</v>
+        <v>8793</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2623,14 +2745,14 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="2">
+      <c r="J41" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>9196</v>
+        <v>9139</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2640,14 +2762,14 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
-      <c r="J42" s="2">
+      <c r="J42" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>9355</v>
+        <v>9196</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2657,14 +2779,14 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
-      <c r="J43" s="2">
+      <c r="J43" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>9516</v>
+        <v>9355</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2674,14 +2796,14 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-      <c r="J44" s="2">
+      <c r="J44" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>9550</v>
+        <v>9516</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2691,14 +2813,14 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-      <c r="J45" s="2">
+      <c r="J45" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>9744</v>
+        <v>9550</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2708,14 +2830,14 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
-      <c r="J46" s="2">
+      <c r="J46" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>9881</v>
+        <v>9744</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2725,206 +2847,223 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
-      <c r="J47" s="2">
+      <c r="J47" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48"/>
+      <c r="A48" s="2">
+        <v>9881</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+      <c r="B49"/>
+    </row>
+    <row r="50" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="10">
+      <c r="B50" s="10">
         <v>50</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C50" s="10">
         <v>50</v>
       </c>
-      <c r="D49" s="10">
+      <c r="D50" s="10">
         <v>50</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E50" s="10">
         <v>50</v>
       </c>
-      <c r="F49" s="10">
+      <c r="F50" s="10">
         <v>50</v>
       </c>
-      <c r="G49" s="10">
+      <c r="G50" s="10">
         <v>50</v>
       </c>
-      <c r="H49" s="10">
+      <c r="H50" s="10">
         <v>50</v>
       </c>
-      <c r="I49" s="10">
+      <c r="I50" s="10">
         <v>50</v>
       </c>
-      <c r="J49" s="11">
+      <c r="J50" s="11">
         <v>1.5</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="12" t="s">
+    <row r="51" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="13" t="e">
-        <f>AVERAGE(B$2:B$47)</f>
+      <c r="B51" s="13" t="e">
+        <f>AVERAGE(B$2:B$48)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C50" s="13" t="e">
-        <f t="shared" ref="C50:J50" si="1">AVERAGE(C$2:C$47)</f>
+      <c r="C51" s="13" t="e">
+        <f t="shared" ref="C51:J51" si="1">AVERAGE(C$2:C$48)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D50" s="13" t="e">
+      <c r="D51" s="13" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E50" s="13" t="e">
+      <c r="E51" s="13" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F50" s="13" t="e">
+      <c r="F51" s="13" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="G50" s="13" t="e">
+      <c r="G51" s="13" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H50" s="13" t="e">
+      <c r="H51" s="13" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I50" s="13" t="e">
+      <c r="I51" s="13" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J50" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" s="13" t="e">
-        <f>STDEV(B$2:B$47)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C51" s="13" t="e">
-        <f t="shared" ref="C51:J51" si="2">STDEV(C$2:C$47)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D51" s="13" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E51" s="13" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F51" s="13" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G51" s="13" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H51" s="13" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I51" s="13" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="J51" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="13" t="e">
+        <f>STDEV(B$2:B$48)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C52" s="13" t="e">
+        <f t="shared" ref="C52:J52" si="2">STDEV(C$2:C$48)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D52" s="13" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E52" s="13" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F52" s="13" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G52" s="13" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H52" s="13" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I52" s="13" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J52" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="13" t="e">
-        <f>MEDIAN(B$2:B$47)</f>
+      <c r="B53" s="13" t="e">
+        <f>MEDIAN(B$2:B$48)</f>
         <v>#NUM!</v>
       </c>
-      <c r="C52" s="13" t="e">
-        <f t="shared" ref="C52:J52" si="3">MEDIAN(C$2:C$47)</f>
+      <c r="C53" s="13" t="e">
+        <f t="shared" ref="C53:J53" si="3">MEDIAN(C$2:C$48)</f>
         <v>#NUM!</v>
       </c>
-      <c r="D52" s="13" t="e">
+      <c r="D53" s="13" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="E52" s="13" t="e">
+      <c r="E53" s="13" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="F52" s="13" t="e">
+      <c r="F53" s="13" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="G52" s="13" t="e">
+      <c r="G53" s="13" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="H52" s="13" t="e">
+      <c r="H53" s="13" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="I52" s="13" t="e">
+      <c r="I53" s="13" t="e">
         <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
-      <c r="J52" s="13">
+      <c r="J53" s="13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="15" t="s">
+    <row r="54" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B53" s="18">
-        <f t="shared" ref="B53:I53" si="4">IF(SUM(B10:B47)&gt;0,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C53" s="16">
+      <c r="B54" s="18">
+        <f t="shared" ref="B54:I54" si="4">IF(SUM(B10:B48)&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C54" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D53" s="16">
+      <c r="D54" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E53" s="16">
+      <c r="E54" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F53" s="16">
+      <c r="F54" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G53" s="16">
+      <c r="G54" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H53" s="16">
+      <c r="H54" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I53" s="16">
+      <c r="I54" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J53" s="10"/>
+      <c r="J54" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2936,10 +3075,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9E2C325-9DED-7647-82A1-46DD08F3F8AF}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3178,157 +3317,164 @@
     </row>
     <row r="33" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>7575</v>
+        <v>7511</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>7642</v>
+        <v>7575</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>7949</v>
+        <v>7642</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>8688</v>
+        <v>7949</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>8742</v>
+        <v>8688</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>8743</v>
+        <v>8742</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
     </row>
     <row r="39" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>8765</v>
+        <v>8743</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>8793</v>
+        <v>8765</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>9139</v>
+        <v>8793</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
     </row>
     <row r="42" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>9196</v>
+        <v>9139</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>9355</v>
+        <v>9196</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>9516</v>
+        <v>9355</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
     </row>
     <row r="45" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>9550</v>
+        <v>9516</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
     <row r="46" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>9744</v>
+        <v>9550</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
     <row r="47" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>9881</v>
+        <v>9744</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+    <row r="48" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>9881</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="20">
+      <c r="B50" s="20">
         <v>100</v>
       </c>
-      <c r="C49" s="20">
+      <c r="C50" s="20">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="12" t="s">
+    <row r="51" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="19" t="e">
-        <f>AVERAGE(B$2:B$47)</f>
+      <c r="B51" s="19" t="e">
+        <f>AVERAGE(B$2:B$48)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C50" s="19" t="e">
-        <f t="shared" ref="C50" si="0">AVERAGE(C$2:C$47)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" s="19" t="e">
-        <f>STDEV(B$2:B$47)</f>
-        <v>#DIV/0!</v>
-      </c>
       <c r="C51" s="19" t="e">
-        <f t="shared" ref="C51" si="1">STDEV(C$2:C$47)</f>
+        <f t="shared" ref="C51" si="0">AVERAGE(C$2:C$48)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="19" t="e">
+        <f>STDEV(B$2:B$48)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C52" s="19" t="e">
+        <f t="shared" ref="C52" si="1">STDEV(C$2:C$48)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="19" t="e">
-        <f>MEDIAN(B$2:B$47)</f>
+      <c r="B53" s="19" t="e">
+        <f>MEDIAN(B$2:B$48)</f>
         <v>#NUM!</v>
       </c>
-      <c r="C52" s="19" t="e">
-        <f t="shared" ref="C52" si="2">MEDIAN(C$2:C$47)</f>
+      <c r="C53" s="19" t="e">
+        <f t="shared" ref="C53" si="2">MEDIAN(C$2:C$48)</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -3342,9 +3488,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279D72AB-081C-F944-AC06-2660F6476096}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -3385,9 +3531,9 @@
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="26">
-        <f>Quizzes!B2</f>
-        <v>0</v>
+      <c r="B2" s="30">
+        <f>Quizzes!L2</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C2" s="26">
         <f>Homeworks!J2</f>
@@ -3401,13 +3547,13 @@
         <f>Exams!C2</f>
         <v>0</v>
       </c>
-      <c r="F2" s="26">
-        <f>$B2+$C2+IF(($E2/$E$49&gt;$D2/$D$49),($E2/$E$49)*7.5, ($D2/$D$49)*3+($E2/$E$49)*4.5)</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="26">
+      <c r="F2" s="30">
+        <f>$B2+$C2+IF(($E2/$E$50&gt;$D2/$D$50),($E2/$E$50)*7.5, ($D2/$D$50)*3+($E2/$E$50)*4.5)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G2" s="31">
         <f>0.5*INT(F2/0.5)+INT( ((F2-INT(F2/0.5)*0.5)/0.25))*0.5</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H2" s="26">
         <f>IF(G2&gt;4.75,1,0)</f>
@@ -3418,9 +3564,9 @@
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="26">
-        <f>Quizzes!B3</f>
-        <v>0</v>
+      <c r="B3" s="30">
+        <f>Quizzes!L3</f>
+        <v>0.46666666666666667</v>
       </c>
       <c r="C3" s="26">
         <f>Homeworks!J3</f>
@@ -3434,16 +3580,16 @@
         <f>Exams!C3</f>
         <v>0</v>
       </c>
-      <c r="F3" s="26">
-        <f t="shared" ref="F3:F47" si="0">$B3+$C3+IF(($E3/$E$49&gt;$D3/$D$49),($E3/$E$49)*7.5, ($D3/$D$49)*3+($E3/$E$49)*4.5)</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="26">
-        <f t="shared" ref="G3:G47" si="1">0.5*INT(F3/0.5)+INT( ((F3-INT(F3/0.5)*0.5)/0.25))*0.5</f>
-        <v>0</v>
+      <c r="F3" s="30">
+        <f t="shared" ref="F3:F48" si="0">$B3+$C3+IF(($E3/$E$50&gt;$D3/$D$50),($E3/$E$50)*7.5, ($D3/$D$50)*3+($E3/$E$50)*4.5)</f>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="G3" s="31">
+        <f t="shared" ref="G3:G48" si="1">0.5*INT(F3/0.5)+INT( ((F3-INT(F3/0.5)*0.5)/0.25))*0.5</f>
+        <v>0.5</v>
       </c>
       <c r="H3" s="26">
-        <f t="shared" ref="H3:H47" si="2">IF(G3&gt;4.75,1,0)</f>
+        <f t="shared" ref="H3:H48" si="2">IF(G3&gt;4.75,1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -3451,9 +3597,9 @@
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="26">
-        <f>Quizzes!B4</f>
-        <v>0</v>
+      <c r="B4" s="30">
+        <f>Quizzes!L4</f>
+        <v>0.73333333333333328</v>
       </c>
       <c r="C4" s="26">
         <f>Homeworks!J4</f>
@@ -3467,13 +3613,13 @@
         <f>Exams!C4</f>
         <v>0</v>
       </c>
-      <c r="F4" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G4" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F4" s="30">
+        <f t="shared" si="0"/>
+        <v>0.73333333333333328</v>
+      </c>
+      <c r="G4" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H4" s="26">
         <f t="shared" si="2"/>
@@ -3484,9 +3630,9 @@
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="26">
-        <f>Quizzes!B5</f>
-        <v>0</v>
+      <c r="B5" s="30">
+        <f>Quizzes!L5</f>
+        <v>0.13333333333333333</v>
       </c>
       <c r="C5" s="26">
         <f>Homeworks!J5</f>
@@ -3500,11 +3646,11 @@
         <f>Exams!C5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="26">
+      <c r="F5" s="30">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="G5" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3517,9 +3663,9 @@
       <c r="A6" s="2">
         <v>1670</v>
       </c>
-      <c r="B6" s="26">
-        <f>Quizzes!B6</f>
-        <v>0</v>
+      <c r="B6" s="30">
+        <f>Quizzes!L6</f>
+        <v>0.73333333333333328</v>
       </c>
       <c r="C6" s="26">
         <f>Homeworks!J6</f>
@@ -3533,13 +3679,13 @@
         <f>Exams!C6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F6" s="30">
+        <f t="shared" si="0"/>
+        <v>0.73333333333333328</v>
+      </c>
+      <c r="G6" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H6" s="26">
         <f t="shared" si="2"/>
@@ -3550,9 +3696,9 @@
       <c r="A7" s="2">
         <v>1691</v>
       </c>
-      <c r="B7" s="26">
-        <f>Quizzes!B7</f>
-        <v>0</v>
+      <c r="B7" s="30">
+        <f>Quizzes!L7</f>
+        <v>0.2</v>
       </c>
       <c r="C7" s="26">
         <f>Homeworks!J7</f>
@@ -3566,11 +3712,11 @@
         <f>Exams!C7</f>
         <v>0</v>
       </c>
-      <c r="F7" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="26">
+      <c r="F7" s="30">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G7" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3583,9 +3729,9 @@
       <c r="A8" s="2">
         <v>1889</v>
       </c>
-      <c r="B8" s="26">
-        <f>Quizzes!B8</f>
-        <v>0</v>
+      <c r="B8" s="30">
+        <f>Quizzes!L8</f>
+        <v>0.13333333333333333</v>
       </c>
       <c r="C8" s="26">
         <f>Homeworks!J8</f>
@@ -3599,11 +3745,11 @@
         <f>Exams!C8</f>
         <v>0</v>
       </c>
-      <c r="F8" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="26">
+      <c r="F8" s="30">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="G8" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3616,9 +3762,9 @@
       <c r="A9" s="2">
         <v>2085</v>
       </c>
-      <c r="B9" s="26">
-        <f>Quizzes!B9</f>
-        <v>0</v>
+      <c r="B9" s="30">
+        <f>Quizzes!L9</f>
+        <v>0.2</v>
       </c>
       <c r="C9" s="26">
         <f>Homeworks!J9</f>
@@ -3632,11 +3778,11 @@
         <f>Exams!C9</f>
         <v>0</v>
       </c>
-      <c r="F9" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="26">
+      <c r="F9" s="30">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G9" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3649,9 +3795,9 @@
       <c r="A10" s="2">
         <v>2163</v>
       </c>
-      <c r="B10" s="26">
-        <f>Quizzes!B10</f>
-        <v>0</v>
+      <c r="B10" s="30">
+        <f>Quizzes!L10</f>
+        <v>0.26666666666666666</v>
       </c>
       <c r="C10" s="26">
         <f>Homeworks!J10</f>
@@ -3665,13 +3811,13 @@
         <f>Exams!C10</f>
         <v>0</v>
       </c>
-      <c r="F10" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F10" s="30">
+        <f t="shared" si="0"/>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="G10" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H10" s="26">
         <f t="shared" si="2"/>
@@ -3682,9 +3828,9 @@
       <c r="A11" s="2">
         <v>2393</v>
       </c>
-      <c r="B11" s="26">
-        <f>Quizzes!B11</f>
-        <v>0</v>
+      <c r="B11" s="30">
+        <f>Quizzes!L11</f>
+        <v>0.53333333333333333</v>
       </c>
       <c r="C11" s="26">
         <f>Homeworks!J11</f>
@@ -3698,13 +3844,13 @@
         <f>Exams!C11</f>
         <v>0</v>
       </c>
-      <c r="F11" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F11" s="30">
+        <f t="shared" si="0"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="G11" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H11" s="26">
         <f t="shared" si="2"/>
@@ -3715,9 +3861,9 @@
       <c r="A12" s="2">
         <v>2441</v>
       </c>
-      <c r="B12" s="26">
-        <f>Quizzes!B12</f>
-        <v>0</v>
+      <c r="B12" s="30">
+        <f>Quizzes!L12</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C12" s="26">
         <f>Homeworks!J12</f>
@@ -3731,13 +3877,13 @@
         <f>Exams!C12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F12" s="30">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G12" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H12" s="26">
         <f t="shared" si="2"/>
@@ -3748,9 +3894,9 @@
       <c r="A13" s="2">
         <v>2903</v>
       </c>
-      <c r="B13" s="26">
-        <f>Quizzes!B13</f>
-        <v>0</v>
+      <c r="B13" s="30">
+        <f>Quizzes!L13</f>
+        <v>0.2</v>
       </c>
       <c r="C13" s="26">
         <f>Homeworks!J13</f>
@@ -3764,11 +3910,11 @@
         <f>Exams!C13</f>
         <v>0</v>
       </c>
-      <c r="F13" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="26">
+      <c r="F13" s="30">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G13" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3781,9 +3927,9 @@
       <c r="A14" s="2">
         <v>2994</v>
       </c>
-      <c r="B14" s="26">
-        <f>Quizzes!B14</f>
-        <v>0</v>
+      <c r="B14" s="30">
+        <f>Quizzes!L14</f>
+        <v>0.46666666666666667</v>
       </c>
       <c r="C14" s="26">
         <f>Homeworks!J14</f>
@@ -3797,13 +3943,13 @@
         <f>Exams!C14</f>
         <v>0</v>
       </c>
-      <c r="F14" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F14" s="30">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="G14" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H14" s="26">
         <f t="shared" si="2"/>
@@ -3814,9 +3960,9 @@
       <c r="A15" s="2">
         <v>3377</v>
       </c>
-      <c r="B15" s="26">
-        <f>Quizzes!B15</f>
-        <v>0</v>
+      <c r="B15" s="30">
+        <f>Quizzes!L15</f>
+        <v>0.4</v>
       </c>
       <c r="C15" s="26">
         <f>Homeworks!J15</f>
@@ -3830,13 +3976,13 @@
         <f>Exams!C15</f>
         <v>0</v>
       </c>
-      <c r="F15" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F15" s="30">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="G15" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H15" s="26">
         <f t="shared" si="2"/>
@@ -3847,9 +3993,9 @@
       <c r="A16" s="2">
         <v>3517</v>
       </c>
-      <c r="B16" s="26">
-        <f>Quizzes!B16</f>
-        <v>0</v>
+      <c r="B16" s="30">
+        <f>Quizzes!L16</f>
+        <v>0.53333333333333333</v>
       </c>
       <c r="C16" s="26">
         <f>Homeworks!J16</f>
@@ -3863,13 +4009,13 @@
         <f>Exams!C16</f>
         <v>0</v>
       </c>
-      <c r="F16" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F16" s="30">
+        <f t="shared" si="0"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="G16" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H16" s="26">
         <f t="shared" si="2"/>
@@ -3880,9 +4026,9 @@
       <c r="A17" s="2">
         <v>3560</v>
       </c>
-      <c r="B17" s="26">
-        <f>Quizzes!B17</f>
-        <v>0</v>
+      <c r="B17" s="30">
+        <f>Quizzes!L17</f>
+        <v>0.46666666666666667</v>
       </c>
       <c r="C17" s="26">
         <f>Homeworks!J17</f>
@@ -3896,13 +4042,13 @@
         <f>Exams!C17</f>
         <v>0</v>
       </c>
-      <c r="F17" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F17" s="30">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="G17" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H17" s="26">
         <f t="shared" si="2"/>
@@ -3913,8 +4059,8 @@
       <c r="A18" s="2">
         <v>3601</v>
       </c>
-      <c r="B18" s="26">
-        <f>Quizzes!B18</f>
+      <c r="B18" s="30">
+        <f>Quizzes!L18</f>
         <v>0</v>
       </c>
       <c r="C18" s="26">
@@ -3929,11 +4075,11 @@
         <f>Exams!C18</f>
         <v>0</v>
       </c>
-      <c r="F18" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="26">
+      <c r="F18" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3946,9 +4092,9 @@
       <c r="A19" s="2">
         <v>3642</v>
       </c>
-      <c r="B19" s="26">
-        <f>Quizzes!B19</f>
-        <v>0</v>
+      <c r="B19" s="30">
+        <f>Quizzes!L19</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C19" s="26">
         <f>Homeworks!J19</f>
@@ -3962,13 +4108,13 @@
         <f>Exams!C19</f>
         <v>0</v>
       </c>
-      <c r="F19" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F19" s="30">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G19" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H19" s="26">
         <f t="shared" si="2"/>
@@ -3979,9 +4125,9 @@
       <c r="A20" s="2">
         <v>3672</v>
       </c>
-      <c r="B20" s="26">
-        <f>Quizzes!B20</f>
-        <v>0</v>
+      <c r="B20" s="30">
+        <f>Quizzes!L20</f>
+        <v>0.8</v>
       </c>
       <c r="C20" s="26">
         <f>Homeworks!J20</f>
@@ -3995,13 +4141,13 @@
         <f>Exams!C20</f>
         <v>0</v>
       </c>
-      <c r="F20" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F20" s="30">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="G20" s="31">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="H20" s="26">
         <f t="shared" si="2"/>
@@ -4012,9 +4158,9 @@
       <c r="A21" s="2">
         <v>3797</v>
       </c>
-      <c r="B21" s="26">
-        <f>Quizzes!B21</f>
-        <v>0</v>
+      <c r="B21" s="30">
+        <f>Quizzes!L21</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C21" s="26">
         <f>Homeworks!J21</f>
@@ -4028,13 +4174,13 @@
         <f>Exams!C21</f>
         <v>0</v>
       </c>
-      <c r="F21" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F21" s="30">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G21" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H21" s="26">
         <f t="shared" si="2"/>
@@ -4045,9 +4191,9 @@
       <c r="A22" s="2">
         <v>4091</v>
       </c>
-      <c r="B22" s="26">
-        <f>Quizzes!B22</f>
-        <v>0</v>
+      <c r="B22" s="30">
+        <f>Quizzes!L22</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C22" s="26">
         <f>Homeworks!J22</f>
@@ -4061,13 +4207,13 @@
         <f>Exams!C22</f>
         <v>0</v>
       </c>
-      <c r="F22" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F22" s="30">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G22" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H22" s="26">
         <f t="shared" si="2"/>
@@ -4078,8 +4224,8 @@
       <c r="A23" s="2">
         <v>4582</v>
       </c>
-      <c r="B23" s="26">
-        <f>Quizzes!B23</f>
+      <c r="B23" s="30">
+        <f>Quizzes!L23</f>
         <v>0</v>
       </c>
       <c r="C23" s="26">
@@ -4094,11 +4240,11 @@
         <f>Exams!C23</f>
         <v>0</v>
       </c>
-      <c r="F23" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="26">
+      <c r="F23" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4111,9 +4257,9 @@
       <c r="A24" s="2">
         <v>4622</v>
       </c>
-      <c r="B24" s="26">
-        <f>Quizzes!B24</f>
-        <v>0</v>
+      <c r="B24" s="30">
+        <f>Quizzes!L24</f>
+        <v>0.26666666666666666</v>
       </c>
       <c r="C24" s="26">
         <f>Homeworks!J24</f>
@@ -4127,13 +4273,13 @@
         <f>Exams!C24</f>
         <v>0</v>
       </c>
-      <c r="F24" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F24" s="30">
+        <f t="shared" si="0"/>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="G24" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H24" s="26">
         <f t="shared" si="2"/>
@@ -4144,9 +4290,9 @@
       <c r="A25" s="2">
         <v>5075</v>
       </c>
-      <c r="B25" s="26">
-        <f>Quizzes!B25</f>
-        <v>0</v>
+      <c r="B25" s="30">
+        <f>Quizzes!L25</f>
+        <v>0.6</v>
       </c>
       <c r="C25" s="26">
         <f>Homeworks!J25</f>
@@ -4160,13 +4306,13 @@
         <f>Exams!C25</f>
         <v>0</v>
       </c>
-      <c r="F25" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F25" s="30">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="G25" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H25" s="26">
         <f t="shared" si="2"/>
@@ -4177,9 +4323,9 @@
       <c r="A26" s="2">
         <v>5141</v>
       </c>
-      <c r="B26" s="26">
-        <f>Quizzes!B26</f>
-        <v>0</v>
+      <c r="B26" s="30">
+        <f>Quizzes!L26</f>
+        <v>0.46666666666666667</v>
       </c>
       <c r="C26" s="26">
         <f>Homeworks!J26</f>
@@ -4193,13 +4339,13 @@
         <f>Exams!C26</f>
         <v>0</v>
       </c>
-      <c r="F26" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F26" s="30">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="G26" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H26" s="26">
         <f t="shared" si="2"/>
@@ -4210,9 +4356,9 @@
       <c r="A27" s="2">
         <v>5482</v>
       </c>
-      <c r="B27" s="26">
-        <f>Quizzes!B27</f>
-        <v>0</v>
+      <c r="B27" s="30">
+        <f>Quizzes!L27</f>
+        <v>0.2</v>
       </c>
       <c r="C27" s="26">
         <f>Homeworks!J27</f>
@@ -4226,11 +4372,11 @@
         <f>Exams!C27</f>
         <v>0</v>
       </c>
-      <c r="F27" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="26">
+      <c r="F27" s="30">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G27" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4243,9 +4389,9 @@
       <c r="A28" s="2">
         <v>5680</v>
       </c>
-      <c r="B28" s="26">
-        <f>Quizzes!B28</f>
-        <v>0</v>
+      <c r="B28" s="30">
+        <f>Quizzes!L28</f>
+        <v>0.13333333333333333</v>
       </c>
       <c r="C28" s="26">
         <f>Homeworks!J28</f>
@@ -4259,11 +4405,11 @@
         <f>Exams!C28</f>
         <v>0</v>
       </c>
-      <c r="F28" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G28" s="26">
+      <c r="F28" s="30">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="G28" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4276,9 +4422,9 @@
       <c r="A29" s="2">
         <v>5943</v>
       </c>
-      <c r="B29" s="26">
-        <f>Quizzes!B29</f>
-        <v>0</v>
+      <c r="B29" s="30">
+        <f>Quizzes!L29</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C29" s="26">
         <f>Homeworks!J29</f>
@@ -4292,13 +4438,13 @@
         <f>Exams!C29</f>
         <v>0</v>
       </c>
-      <c r="F29" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G29" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F29" s="30">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G29" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H29" s="26">
         <f t="shared" si="2"/>
@@ -4309,9 +4455,9 @@
       <c r="A30" s="2">
         <v>6464</v>
       </c>
-      <c r="B30" s="26">
-        <f>Quizzes!B30</f>
-        <v>0</v>
+      <c r="B30" s="30">
+        <f>Quizzes!L30</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C30" s="26">
         <f>Homeworks!J30</f>
@@ -4325,13 +4471,13 @@
         <f>Exams!C30</f>
         <v>0</v>
       </c>
-      <c r="F30" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F30" s="30">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G30" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H30" s="26">
         <f t="shared" si="2"/>
@@ -4342,9 +4488,9 @@
       <c r="A31" s="2">
         <v>6797</v>
       </c>
-      <c r="B31" s="26">
-        <f>Quizzes!B31</f>
-        <v>0</v>
+      <c r="B31" s="30">
+        <f>Quizzes!L31</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C31" s="26">
         <f>Homeworks!J31</f>
@@ -4358,13 +4504,13 @@
         <f>Exams!C31</f>
         <v>0</v>
       </c>
-      <c r="F31" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G31" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F31" s="30">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G31" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H31" s="26">
         <f t="shared" si="2"/>
@@ -4375,9 +4521,9 @@
       <c r="A32" s="2">
         <v>7021</v>
       </c>
-      <c r="B32" s="26">
-        <f>Quizzes!B32</f>
-        <v>0</v>
+      <c r="B32" s="30">
+        <f>Quizzes!L32</f>
+        <v>0.4</v>
       </c>
       <c r="C32" s="26">
         <f>Homeworks!J32</f>
@@ -4391,13 +4537,13 @@
         <f>Exams!C32</f>
         <v>0</v>
       </c>
-      <c r="F32" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G32" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F32" s="30">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="G32" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H32" s="26">
         <f t="shared" si="2"/>
@@ -4406,10 +4552,10 @@
     </row>
     <row r="33" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>7575</v>
-      </c>
-      <c r="B33" s="26">
-        <f>Quizzes!B33</f>
+        <v>7511</v>
+      </c>
+      <c r="B33" s="30">
+        <f>Quizzes!L33</f>
         <v>0</v>
       </c>
       <c r="C33" s="26">
@@ -4424,26 +4570,26 @@
         <f>Exams!C33</f>
         <v>0</v>
       </c>
-      <c r="F33" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G33" s="26">
-        <f t="shared" si="1"/>
+      <c r="F33" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G33" s="31">
+        <f t="shared" ref="G33" si="3">0.5*INT(F33/0.5)+INT( ((F33-INT(F33/0.5)*0.5)/0.25))*0.5</f>
         <v>0</v>
       </c>
       <c r="H33" s="26">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H33" si="4">IF(G33&gt;4.75,1,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>7642</v>
-      </c>
-      <c r="B34" s="26">
-        <f>Quizzes!B34</f>
-        <v>0</v>
+        <v>7575</v>
+      </c>
+      <c r="B34" s="30">
+        <f>Quizzes!L34</f>
+        <v>0.2</v>
       </c>
       <c r="C34" s="26">
         <f>Homeworks!J34</f>
@@ -4457,11 +4603,11 @@
         <f>Exams!C34</f>
         <v>0</v>
       </c>
-      <c r="F34" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G34" s="26">
+      <c r="F34" s="30">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G34" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4472,11 +4618,11 @@
     </row>
     <row r="35" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>7949</v>
-      </c>
-      <c r="B35" s="26">
-        <f>Quizzes!B35</f>
-        <v>0</v>
+        <v>7642</v>
+      </c>
+      <c r="B35" s="30">
+        <f>Quizzes!L35</f>
+        <v>0.2</v>
       </c>
       <c r="C35" s="26">
         <f>Homeworks!J35</f>
@@ -4490,11 +4636,11 @@
         <f>Exams!C35</f>
         <v>0</v>
       </c>
-      <c r="F35" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G35" s="26">
+      <c r="F35" s="30">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="G35" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4505,10 +4651,10 @@
     </row>
     <row r="36" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>8688</v>
-      </c>
-      <c r="B36" s="26">
-        <f>Quizzes!B36</f>
+        <v>7949</v>
+      </c>
+      <c r="B36" s="30">
+        <f>Quizzes!L36</f>
         <v>0</v>
       </c>
       <c r="C36" s="26">
@@ -4523,11 +4669,11 @@
         <f>Exams!C36</f>
         <v>0</v>
       </c>
-      <c r="F36" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G36" s="26">
+      <c r="F36" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4538,10 +4684,10 @@
     </row>
     <row r="37" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>8742</v>
-      </c>
-      <c r="B37" s="26">
-        <f>Quizzes!B37</f>
+        <v>8688</v>
+      </c>
+      <c r="B37" s="30">
+        <f>Quizzes!L37</f>
         <v>0</v>
       </c>
       <c r="C37" s="26">
@@ -4556,11 +4702,11 @@
         <f>Exams!C37</f>
         <v>0</v>
       </c>
-      <c r="F37" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G37" s="26">
+      <c r="F37" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G37" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4571,11 +4717,11 @@
     </row>
     <row r="38" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>8743</v>
-      </c>
-      <c r="B38" s="26">
-        <f>Quizzes!B38</f>
-        <v>0</v>
+        <v>8742</v>
+      </c>
+      <c r="B38" s="30">
+        <f>Quizzes!L38</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C38" s="26">
         <f>Homeworks!J38</f>
@@ -4589,13 +4735,13 @@
         <f>Exams!C38</f>
         <v>0</v>
       </c>
-      <c r="F38" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G38" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F38" s="30">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G38" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H38" s="26">
         <f t="shared" si="2"/>
@@ -4604,11 +4750,11 @@
     </row>
     <row r="39" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>8765</v>
-      </c>
-      <c r="B39" s="26">
-        <f>Quizzes!B39</f>
-        <v>0</v>
+        <v>8743</v>
+      </c>
+      <c r="B39" s="30">
+        <f>Quizzes!L39</f>
+        <v>0.4</v>
       </c>
       <c r="C39" s="26">
         <f>Homeworks!J39</f>
@@ -4622,13 +4768,13 @@
         <f>Exams!C39</f>
         <v>0</v>
       </c>
-      <c r="F39" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G39" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F39" s="30">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="G39" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H39" s="26">
         <f t="shared" si="2"/>
@@ -4637,11 +4783,11 @@
     </row>
     <row r="40" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>8793</v>
-      </c>
-      <c r="B40" s="26">
-        <f>Quizzes!B40</f>
-        <v>0</v>
+        <v>8765</v>
+      </c>
+      <c r="B40" s="30">
+        <f>Quizzes!L40</f>
+        <v>0.4</v>
       </c>
       <c r="C40" s="26">
         <f>Homeworks!J40</f>
@@ -4655,13 +4801,13 @@
         <f>Exams!C40</f>
         <v>0</v>
       </c>
-      <c r="F40" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G40" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F40" s="30">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="G40" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H40" s="26">
         <f t="shared" si="2"/>
@@ -4670,11 +4816,11 @@
     </row>
     <row r="41" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>9139</v>
-      </c>
-      <c r="B41" s="26">
-        <f>Quizzes!B41</f>
-        <v>0</v>
+        <v>8793</v>
+      </c>
+      <c r="B41" s="30">
+        <f>Quizzes!L41</f>
+        <v>0.53333333333333333</v>
       </c>
       <c r="C41" s="26">
         <f>Homeworks!J41</f>
@@ -4688,13 +4834,13 @@
         <f>Exams!C41</f>
         <v>0</v>
       </c>
-      <c r="F41" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G41" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F41" s="30">
+        <f t="shared" si="0"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="G41" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H41" s="26">
         <f t="shared" si="2"/>
@@ -4703,11 +4849,11 @@
     </row>
     <row r="42" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>9196</v>
-      </c>
-      <c r="B42" s="26">
-        <f>Quizzes!B42</f>
-        <v>0</v>
+        <v>9139</v>
+      </c>
+      <c r="B42" s="30">
+        <f>Quizzes!L42</f>
+        <v>0.13333333333333333</v>
       </c>
       <c r="C42" s="26">
         <f>Homeworks!J42</f>
@@ -4721,11 +4867,11 @@
         <f>Exams!C42</f>
         <v>0</v>
       </c>
-      <c r="F42" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G42" s="26">
+      <c r="F42" s="30">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="G42" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4736,11 +4882,11 @@
     </row>
     <row r="43" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>9355</v>
-      </c>
-      <c r="B43" s="26">
-        <f>Quizzes!B43</f>
-        <v>0</v>
+        <v>9196</v>
+      </c>
+      <c r="B43" s="30">
+        <f>Quizzes!L43</f>
+        <v>0.46666666666666667</v>
       </c>
       <c r="C43" s="26">
         <f>Homeworks!J43</f>
@@ -4754,13 +4900,13 @@
         <f>Exams!C43</f>
         <v>0</v>
       </c>
-      <c r="F43" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G43" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F43" s="30">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="G43" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H43" s="26">
         <f t="shared" si="2"/>
@@ -4769,11 +4915,11 @@
     </row>
     <row r="44" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>9516</v>
-      </c>
-      <c r="B44" s="26">
-        <f>Quizzes!B44</f>
-        <v>0</v>
+        <v>9355</v>
+      </c>
+      <c r="B44" s="30">
+        <f>Quizzes!L44</f>
+        <v>0.53333333333333333</v>
       </c>
       <c r="C44" s="26">
         <f>Homeworks!J44</f>
@@ -4787,13 +4933,13 @@
         <f>Exams!C44</f>
         <v>0</v>
       </c>
-      <c r="F44" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G44" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F44" s="30">
+        <f t="shared" si="0"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="G44" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H44" s="26">
         <f t="shared" si="2"/>
@@ -4802,10 +4948,10 @@
     </row>
     <row r="45" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>9550</v>
-      </c>
-      <c r="B45" s="26">
-        <f>Quizzes!B45</f>
+        <v>9516</v>
+      </c>
+      <c r="B45" s="30">
+        <f>Quizzes!L45</f>
         <v>0</v>
       </c>
       <c r="C45" s="26">
@@ -4820,11 +4966,11 @@
         <f>Exams!C45</f>
         <v>0</v>
       </c>
-      <c r="F45" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G45" s="26">
+      <c r="F45" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G45" s="31">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4835,11 +4981,11 @@
     </row>
     <row r="46" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>9744</v>
-      </c>
-      <c r="B46" s="26">
-        <f>Quizzes!B46</f>
-        <v>0</v>
+        <v>9550</v>
+      </c>
+      <c r="B46" s="30">
+        <f>Quizzes!L46</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C46" s="26">
         <f>Homeworks!J46</f>
@@ -4853,13 +4999,13 @@
         <f>Exams!C46</f>
         <v>0</v>
       </c>
-      <c r="F46" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G46" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F46" s="30">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G46" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H46" s="26">
         <f t="shared" si="2"/>
@@ -4868,11 +5014,11 @@
     </row>
     <row r="47" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>9881</v>
-      </c>
-      <c r="B47" s="26">
-        <f>Quizzes!B47</f>
-        <v>0</v>
+        <v>9744</v>
+      </c>
+      <c r="B47" s="30">
+        <f>Quizzes!L47</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C47" s="26">
         <f>Homeworks!J47</f>
@@ -4886,147 +5032,180 @@
         <f>Exams!C47</f>
         <v>0</v>
       </c>
-      <c r="F47" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G47" s="26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="F47" s="30">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G47" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="H47" s="26">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
+    <row r="48" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>9881</v>
+      </c>
+      <c r="B48" s="30">
+        <f>Quizzes!L48</f>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="C48" s="26">
+        <f>Homeworks!J48</f>
+        <v>0</v>
+      </c>
+      <c r="D48" s="26">
+        <f>Exams!B48</f>
+        <v>0</v>
+      </c>
+      <c r="E48" s="26">
+        <f>Exams!C48</f>
+        <v>0</v>
+      </c>
+      <c r="F48" s="30">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="G48" s="31">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="H48" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="11">
-        <f>Quizzes!L49</f>
+      <c r="B50" s="11">
+        <f>Quizzes!L50</f>
         <v>1</v>
       </c>
-      <c r="C49" s="25">
-        <f>Homeworks!J49</f>
+      <c r="C50" s="25">
+        <f>Homeworks!J50</f>
         <v>1.5</v>
       </c>
-      <c r="D49" s="9">
-        <f>Exams!B49</f>
+      <c r="D50" s="9">
+        <f>Exams!B50</f>
         <v>100</v>
       </c>
-      <c r="E49" s="10">
-        <f>Exams!C49</f>
+      <c r="E50" s="10">
+        <f>Exams!C50</f>
         <v>100</v>
       </c>
-      <c r="F49" s="10">
+      <c r="F50" s="10">
         <v>10</v>
       </c>
-      <c r="G49" s="10">
+      <c r="G50" s="10">
         <v>10</v>
       </c>
-      <c r="H49" s="10">
-        <f>SUM(H2:H47)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="12" t="s">
+      <c r="H50" s="10">
+        <f>SUM(H2:H48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="13">
-        <f>AVERAGE(B$2:B$47)</f>
-        <v>0</v>
-      </c>
-      <c r="C50" s="13">
-        <f t="shared" ref="C50:H50" si="3">AVERAGE(C$2:C$47)</f>
-        <v>0</v>
-      </c>
-      <c r="D50" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E50" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F50" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G50" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H50" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
-        <v>18</v>
-      </c>
       <c r="B51" s="13">
-        <f>STDEV(B$2:B$47)</f>
-        <v>0</v>
+        <f>AVERAGE(B$2:B$48)</f>
+        <v>0.36170212765957438</v>
       </c>
       <c r="C51" s="13">
-        <f t="shared" ref="C51:H51" si="4">STDEV(C$2:C$47)</f>
+        <f t="shared" ref="C51:H51" si="5">AVERAGE(C$2:C$48)</f>
         <v>0</v>
       </c>
       <c r="D51" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E51" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F51" s="13">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0.36170212765957438</v>
       </c>
       <c r="G51" s="13">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0.34042553191489361</v>
       </c>
       <c r="H51" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" s="13">
+        <f>STDEV(B$2:B$48)</f>
+        <v>0.22618221069524505</v>
+      </c>
+      <c r="C52" s="13">
+        <f t="shared" ref="C52:H52" si="6">STDEV(C$2:C$48)</f>
+        <v>0</v>
+      </c>
+      <c r="D52" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="13">
+        <f t="shared" si="6"/>
+        <v>0.22618221069524505</v>
+      </c>
+      <c r="G52" s="13">
+        <f t="shared" si="6"/>
+        <v>0.25763099198194733</v>
+      </c>
+      <c r="H52" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="13">
-        <f>MEDIAN(B$2:B$47)</f>
-        <v>0</v>
-      </c>
-      <c r="C52" s="13">
-        <f t="shared" ref="C52:H52" si="5">MEDIAN(C$2:C$47)</f>
-        <v>0</v>
-      </c>
-      <c r="D52" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="E52" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F52" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G52" s="13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H52" s="13">
-        <f t="shared" si="5"/>
+      <c r="B53" s="13">
+        <f>MEDIAN(B$2:B$48)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C53" s="13">
+        <f t="shared" ref="C53:H53" si="7">MEDIAN(C$2:C$48)</f>
+        <v>0</v>
+      </c>
+      <c r="D53" s="13">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E53" s="13">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="13">
+        <f t="shared" si="7"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G53" s="13">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="H53" s="13">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes HM07 and HM08
</commit_message>
<xml_diff>
--- a/phy140/Grades/grades_report_2023.xlsx
+++ b/phy140/Grades/grades_report_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ptohos/Documents/MyCourses/FYS140/2023/Grades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5954F260-CBD5-2848-9FD2-1E37FF74C3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6EDA45-7A97-0A44-8463-26A5BC6CFD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5520" yWindow="1680" windowWidth="30320" windowHeight="20720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2770,11 +2770,15 @@
       <c r="G2" s="27">
         <v>0</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="H2" s="27">
+        <v>0</v>
+      </c>
+      <c r="I2" s="27">
+        <v>0</v>
+      </c>
       <c r="J2" s="27">
         <f t="shared" ref="J2:J48" si="0">IF(SUM($B$54:$I$54)&gt;0,$J$50*(B2/$B$50+C2/$C$50+D2/$D$50+E2/$E$50+F2/$F$50+G2/$G$50+H2/$H$50+I2/$I$50)/SUM($B$54:$I$54),0)</f>
-        <v>0.03</v>
+        <v>2.2499999999999999E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2799,11 +2803,15 @@
       <c r="G3" s="27">
         <v>36.5</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="H3" s="27">
+        <v>56</v>
+      </c>
+      <c r="I3" s="27">
+        <v>68</v>
+      </c>
       <c r="J3" s="27">
         <f t="shared" si="0"/>
-        <v>1.2193749999999999</v>
+        <v>1.2716741071428572</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2828,11 +2836,15 @@
       <c r="G4" s="27">
         <v>45.5</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="H4" s="27">
+        <v>60</v>
+      </c>
+      <c r="I4" s="27">
+        <v>70</v>
+      </c>
       <c r="J4" s="27">
         <f t="shared" si="0"/>
-        <v>1.39671875</v>
+        <v>1.4225390625000001</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2857,11 +2869,15 @@
       <c r="G5" s="27">
         <v>0</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="H5" s="27">
+        <v>0</v>
+      </c>
+      <c r="I5" s="27">
+        <v>0</v>
+      </c>
       <c r="J5" s="27">
         <f t="shared" si="0"/>
-        <v>0.20000000000000004</v>
+        <v>0.15000000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2886,11 +2902,15 @@
       <c r="G6" s="27">
         <v>0</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="H6" s="27">
+        <v>0</v>
+      </c>
+      <c r="I6" s="27">
+        <v>0</v>
+      </c>
       <c r="J6" s="27">
         <f t="shared" si="0"/>
-        <v>0.45218749999999996</v>
+        <v>0.33914062499999997</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2915,11 +2935,15 @@
       <c r="G7" s="27">
         <v>27</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="H7" s="27">
+        <v>57</v>
+      </c>
+      <c r="I7" s="27">
+        <v>57.5</v>
+      </c>
       <c r="J7" s="27">
         <f t="shared" si="0"/>
-        <v>0.70874999999999988</v>
+        <v>0.86370535714285712</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2944,11 +2968,15 @@
       <c r="G8" s="27">
         <v>0</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="H8" s="27">
+        <v>0</v>
+      </c>
+      <c r="I8" s="27">
+        <v>3</v>
+      </c>
       <c r="J8" s="27">
         <f t="shared" si="0"/>
-        <v>2.5000000000000005E-2</v>
+        <v>2.6785714285714284E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2973,11 +3001,15 @@
       <c r="G9" s="27">
         <v>3</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="H9" s="27">
+        <v>17</v>
+      </c>
+      <c r="I9" s="27">
+        <v>0</v>
+      </c>
       <c r="J9" s="27">
         <f t="shared" si="0"/>
-        <v>0.44968750000000002</v>
+        <v>0.39039062499999999</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3002,11 +3034,15 @@
       <c r="G10" s="27">
         <v>40.5</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="H10" s="27">
+        <v>58.5</v>
+      </c>
+      <c r="I10" s="27">
+        <v>67</v>
+      </c>
       <c r="J10" s="27">
         <f t="shared" si="0"/>
-        <v>1.3321874999999999</v>
+        <v>1.3614174107142856</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3031,11 +3067,15 @@
       <c r="G11" s="27">
         <v>0</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="H11" s="27">
+        <v>0</v>
+      </c>
+      <c r="I11" s="27">
+        <v>0</v>
+      </c>
       <c r="J11" s="27">
         <f t="shared" si="0"/>
-        <v>0.14250000000000002</v>
+        <v>0.10687500000000001</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3060,11 +3100,15 @@
       <c r="G12" s="27">
         <v>32.5</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="H12" s="27">
+        <v>0</v>
+      </c>
+      <c r="I12" s="27">
+        <v>66</v>
+      </c>
       <c r="J12" s="27">
         <f t="shared" si="0"/>
-        <v>1.1681250000000001</v>
+        <v>1.0528794642857144</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3089,11 +3133,15 @@
       <c r="G13" s="27">
         <v>32</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="H13" s="27">
+        <v>52</v>
+      </c>
+      <c r="I13" s="27">
+        <v>59</v>
+      </c>
       <c r="J13" s="27">
         <f t="shared" si="0"/>
-        <v>0.94781250000000006</v>
+        <v>1.0313950892857142</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3118,11 +3166,15 @@
       <c r="G14" s="27">
         <v>21.5</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="H14" s="27">
+        <v>30</v>
+      </c>
+      <c r="I14" s="27">
+        <v>0</v>
+      </c>
       <c r="J14" s="27">
         <f t="shared" si="0"/>
-        <v>0.52687500000000009</v>
+        <v>0.4889062500000001</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3147,11 +3199,15 @@
       <c r="G15" s="27">
         <v>21.5</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="H15" s="27">
+        <v>38.5</v>
+      </c>
+      <c r="I15" s="27">
+        <v>54</v>
+      </c>
       <c r="J15" s="27">
         <f t="shared" si="0"/>
-        <v>0.66156250000000005</v>
+        <v>0.76112723214285716</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3176,11 +3232,15 @@
       <c r="G16" s="27">
         <v>36</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="H16" s="27">
+        <v>48</v>
+      </c>
+      <c r="I16" s="27">
+        <v>48</v>
+      </c>
       <c r="J16" s="27">
         <f t="shared" si="0"/>
-        <v>1.2110937500000001</v>
+        <v>1.1868917410714286</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3205,11 +3265,15 @@
       <c r="G17" s="27">
         <v>29.5</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="H17" s="27">
+        <v>50.5</v>
+      </c>
+      <c r="I17" s="27">
+        <v>56.5</v>
+      </c>
       <c r="J17" s="27">
         <f t="shared" si="0"/>
-        <v>0.54812499999999997</v>
+        <v>0.72024553571428562</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3234,11 +3298,15 @@
       <c r="G18" s="27">
         <v>0</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="H18" s="27">
+        <v>0</v>
+      </c>
+      <c r="I18" s="27">
+        <v>0</v>
+      </c>
       <c r="J18" s="27">
         <f t="shared" si="0"/>
-        <v>0.10843750000000001</v>
+        <v>8.1328125000000001E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3263,11 +3331,15 @@
       <c r="G19" s="27">
         <v>30</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="H19" s="27">
+        <v>53.5</v>
+      </c>
+      <c r="I19" s="27">
+        <v>59</v>
+      </c>
       <c r="J19" s="27">
         <f t="shared" si="0"/>
-        <v>1.09765625</v>
+        <v>1.1484654017857143</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3292,11 +3364,15 @@
       <c r="G20" s="27">
         <v>30.5</v>
       </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="H20" s="27">
+        <v>54</v>
+      </c>
+      <c r="I20" s="27">
+        <v>64</v>
+      </c>
       <c r="J20" s="27">
         <f t="shared" si="0"/>
-        <v>1.05078125</v>
+        <v>1.1282645089285714</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3321,11 +3397,15 @@
       <c r="G21" s="27">
         <v>21.5</v>
       </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="H21" s="27">
+        <v>30</v>
+      </c>
+      <c r="I21" s="27">
+        <v>27</v>
+      </c>
       <c r="J21" s="27">
         <f t="shared" si="0"/>
-        <v>0.93437500000000007</v>
+        <v>0.86685267857142878</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3350,11 +3430,15 @@
       <c r="G22" s="27">
         <v>46</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="H22" s="27">
+        <v>60</v>
+      </c>
+      <c r="I22" s="27">
+        <v>67</v>
+      </c>
       <c r="J22" s="27">
         <f t="shared" si="0"/>
-        <v>1.3451562499999998</v>
+        <v>1.3758314732142858</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3377,13 +3461,17 @@
         <v>37.5</v>
       </c>
       <c r="G23" s="27">
-        <v>28</v>
-      </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="H23" s="27">
+        <v>42.5</v>
+      </c>
+      <c r="I23" s="27">
+        <v>0</v>
+      </c>
       <c r="J23" s="27">
         <f t="shared" si="0"/>
-        <v>1.0618750000000001</v>
+        <v>0.95171874999999995</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3408,11 +3496,15 @@
       <c r="G24" s="27">
         <v>10</v>
       </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+      <c r="H24" s="27">
+        <v>22</v>
+      </c>
+      <c r="I24" s="27">
+        <v>48.5</v>
+      </c>
       <c r="J24" s="27">
         <f t="shared" si="0"/>
-        <v>0.54937500000000006</v>
+        <v>0.61069196428571437</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3437,11 +3529,15 @@
       <c r="G25" s="27">
         <v>33.5</v>
       </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
+      <c r="H25" s="27">
+        <v>31</v>
+      </c>
+      <c r="I25" s="27">
+        <v>43</v>
+      </c>
       <c r="J25" s="27">
         <f t="shared" si="0"/>
-        <v>0.50593750000000004</v>
+        <v>0.59150669642857145</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3466,11 +3562,15 @@
       <c r="G26" s="27">
         <v>14</v>
       </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+      <c r="H26" s="27">
+        <v>44.5</v>
+      </c>
+      <c r="I26" s="27">
+        <v>68</v>
+      </c>
       <c r="J26" s="27">
         <f t="shared" si="0"/>
-        <v>0.56812499999999999</v>
+        <v>0.74729910714285719</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3495,11 +3595,15 @@
       <c r="G27" s="27">
         <v>0</v>
       </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="H27" s="27">
+        <v>24</v>
+      </c>
+      <c r="I27" s="27">
+        <v>44</v>
+      </c>
       <c r="J27" s="27">
         <f t="shared" si="0"/>
-        <v>0.54953125000000003</v>
+        <v>0.6050055803571428</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3524,11 +3628,15 @@
       <c r="G28" s="27">
         <v>7</v>
       </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="H28" s="27">
+        <v>0</v>
+      </c>
+      <c r="I28" s="27">
+        <v>17.5</v>
+      </c>
       <c r="J28" s="27">
         <f t="shared" si="0"/>
-        <v>8.8125000000000009E-2</v>
+        <v>0.11296875000000001</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3553,11 +3661,15 @@
       <c r="G29" s="27">
         <v>18</v>
       </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
+      <c r="H29" s="27">
+        <v>18</v>
+      </c>
+      <c r="I29" s="27">
+        <v>31.5</v>
+      </c>
       <c r="J29" s="27">
         <f t="shared" si="0"/>
-        <v>0.19499999999999998</v>
+        <v>0.28687499999999999</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3582,11 +3694,15 @@
       <c r="G30" s="27">
         <v>44</v>
       </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
+      <c r="H30" s="27">
+        <v>53.5</v>
+      </c>
+      <c r="I30" s="27">
+        <v>62</v>
+      </c>
       <c r="J30" s="27">
         <f t="shared" si="0"/>
-        <v>1.41</v>
+        <v>1.3907589285714286</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3611,11 +3727,15 @@
       <c r="G31" s="27">
         <v>10</v>
       </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
+      <c r="H31" s="27">
+        <v>39.5</v>
+      </c>
+      <c r="I31" s="27">
+        <v>48</v>
+      </c>
       <c r="J31" s="27">
         <f t="shared" si="0"/>
-        <v>0.75546875000000002</v>
+        <v>0.81861049107142869</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3640,11 +3760,15 @@
       <c r="G32" s="27">
         <v>0</v>
       </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
+      <c r="H32" s="27">
+        <v>42</v>
+      </c>
+      <c r="I32" s="27">
+        <v>44.5</v>
+      </c>
       <c r="J32" s="27">
         <f t="shared" si="0"/>
-        <v>0.82281249999999995</v>
+        <v>0.86755580357142847</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3669,8 +3793,12 @@
       <c r="G33" s="27">
         <v>0</v>
       </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
+      <c r="H33" s="27">
+        <v>0</v>
+      </c>
+      <c r="I33" s="27">
+        <v>0</v>
+      </c>
       <c r="J33" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3698,11 +3826,15 @@
       <c r="G34" s="27">
         <v>20.5</v>
       </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
+      <c r="H34" s="27">
+        <v>28</v>
+      </c>
+      <c r="I34" s="27">
+        <v>44.5</v>
+      </c>
       <c r="J34" s="27">
         <f t="shared" si="0"/>
-        <v>0.62375000000000003</v>
+        <v>0.67450892857142863</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3727,11 +3859,15 @@
       <c r="G35" s="27">
         <v>0</v>
       </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
+      <c r="H35" s="27">
+        <v>0</v>
+      </c>
+      <c r="I35" s="27">
+        <v>9</v>
+      </c>
       <c r="J35" s="27">
         <f t="shared" si="0"/>
-        <v>0.19187499999999999</v>
+        <v>0.16801339285714284</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3756,8 +3892,12 @@
       <c r="G36" s="27">
         <v>0</v>
       </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
+      <c r="H36" s="27">
+        <v>0</v>
+      </c>
+      <c r="I36" s="27">
+        <v>0</v>
+      </c>
       <c r="J36" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3785,8 +3925,12 @@
       <c r="G37" s="27">
         <v>0</v>
       </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
+      <c r="H37" s="27">
+        <v>0</v>
+      </c>
+      <c r="I37" s="27">
+        <v>0</v>
+      </c>
       <c r="J37" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3814,11 +3958,15 @@
       <c r="G38" s="27">
         <v>30</v>
       </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
+      <c r="H38" s="27">
+        <v>35</v>
+      </c>
+      <c r="I38" s="27">
+        <v>58</v>
+      </c>
       <c r="J38" s="27">
         <f t="shared" si="0"/>
-        <v>0.55562500000000004</v>
+        <v>0.681450892857143</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3843,11 +3991,15 @@
       <c r="G39" s="27">
         <v>0</v>
       </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
+      <c r="H39" s="27">
+        <v>0</v>
+      </c>
+      <c r="I39" s="27">
+        <v>33</v>
+      </c>
       <c r="J39" s="27">
         <f t="shared" si="0"/>
-        <v>0.75749999999999995</v>
+        <v>0.65651785714285715</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3872,11 +4024,15 @@
       <c r="G40" s="27">
         <v>12.5</v>
       </c>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
+      <c r="H40" s="27">
+        <v>31</v>
+      </c>
+      <c r="I40" s="27">
+        <v>45</v>
+      </c>
       <c r="J40" s="27">
         <f t="shared" si="0"/>
-        <v>0.22437499999999999</v>
+        <v>0.38569196428571428</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3901,11 +4057,15 @@
       <c r="G41" s="27">
         <v>42.5</v>
       </c>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
+      <c r="H41" s="27">
+        <v>60</v>
+      </c>
+      <c r="I41" s="27">
+        <v>64</v>
+      </c>
       <c r="J41" s="27">
         <f t="shared" si="0"/>
-        <v>1.34078125</v>
+        <v>1.3645145089285715</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3930,11 +4090,15 @@
       <c r="G42" s="27">
         <v>5</v>
       </c>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
+      <c r="H42" s="27">
+        <v>42</v>
+      </c>
+      <c r="I42" s="27">
+        <v>56.5</v>
+      </c>
       <c r="J42" s="27">
         <f t="shared" si="0"/>
-        <v>0.26375000000000004</v>
+        <v>0.48040178571428571</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3959,11 +4123,15 @@
       <c r="G43" s="27">
         <v>39</v>
       </c>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
+      <c r="H43" s="27">
+        <v>59.5</v>
+      </c>
+      <c r="I43" s="27">
+        <v>59.5</v>
+      </c>
       <c r="J43" s="27">
         <f t="shared" si="0"/>
-        <v>1.1612500000000001</v>
+        <v>1.2162500000000001</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3988,11 +4156,15 @@
       <c r="G44" s="27">
         <v>39</v>
       </c>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
+      <c r="H44" s="27">
+        <v>52.5</v>
+      </c>
+      <c r="I44" s="27">
+        <v>67.5</v>
+      </c>
       <c r="J44" s="27">
         <f t="shared" si="0"/>
-        <v>0.92937499999999995</v>
+        <v>1.0418973214285714</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4017,8 +4189,12 @@
       <c r="G45" s="27">
         <v>0</v>
       </c>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
+      <c r="H45" s="27">
+        <v>0</v>
+      </c>
+      <c r="I45" s="27">
+        <v>0</v>
+      </c>
       <c r="J45" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4046,11 +4222,15 @@
       <c r="G46" s="27">
         <v>32.5</v>
       </c>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
+      <c r="H46" s="27">
+        <v>50</v>
+      </c>
+      <c r="I46" s="27">
+        <v>45</v>
+      </c>
       <c r="J46" s="27">
         <f t="shared" si="0"/>
-        <v>0.81859375000000012</v>
+        <v>0.89073102678571425</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4075,11 +4255,15 @@
       <c r="G47" s="27">
         <v>0</v>
       </c>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
+      <c r="H47" s="27">
+        <v>0</v>
+      </c>
+      <c r="I47" s="27">
+        <v>0</v>
+      </c>
       <c r="J47" s="27">
         <f t="shared" si="0"/>
-        <v>0.34703124999999996</v>
+        <v>0.26027343749999998</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4104,11 +4288,15 @@
       <c r="G48" s="27">
         <v>0</v>
       </c>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
+      <c r="H48" s="27">
+        <v>0</v>
+      </c>
+      <c r="I48" s="27">
+        <v>0</v>
+      </c>
       <c r="J48" s="27">
         <f t="shared" si="0"/>
-        <v>0.21406249999999996</v>
+        <v>0.16054687499999998</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4172,19 +4360,19 @@
       </c>
       <c r="G51" s="13">
         <f t="shared" si="1"/>
-        <v>17.851063829787233</v>
-      </c>
-      <c r="H51" s="13" t="e">
+        <v>17.978723404255319</v>
+      </c>
+      <c r="H51" s="13">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I51" s="13" t="e">
+        <v>28.51063829787234</v>
+      </c>
+      <c r="I51" s="13">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>35.212765957446805</v>
       </c>
       <c r="J51" s="13">
         <f t="shared" si="1"/>
-        <v>0.62746010638297889</v>
+        <v>0.65448945668693015</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4213,19 +4401,19 @@
       </c>
       <c r="G52" s="13">
         <f t="shared" si="2"/>
-        <v>16.41874422381753</v>
-      </c>
-      <c r="H52" s="13" t="e">
+        <v>16.522368713356222</v>
+      </c>
+      <c r="H52" s="13">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I52" s="13" t="e">
+        <v>23.386750560042152</v>
+      </c>
+      <c r="I52" s="13">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>27.279699547475868</v>
       </c>
       <c r="J52" s="13">
         <f t="shared" si="2"/>
-        <v>0.44949257777572238</v>
+        <v>0.45797216731590284</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4256,17 +4444,17 @@
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="H53" s="13" t="e">
+      <c r="H53" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="I53" s="13" t="e">
+        <v>31</v>
+      </c>
+      <c r="I53" s="13">
         <f t="shared" si="3"/>
-        <v>#NUM!</v>
+        <v>44.5</v>
       </c>
       <c r="J53" s="13">
         <f t="shared" si="3"/>
-        <v>0.55562500000000004</v>
+        <v>0.67450892857142863</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -4299,11 +4487,11 @@
       </c>
       <c r="H54" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54" s="16">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54" s="10"/>
     </row>
@@ -4909,7 +5097,7 @@
       </c>
       <c r="C2" s="28">
         <f>Homeworks!J2</f>
-        <v>0.03</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="D2" s="26">
         <f>Exams!B2</f>
@@ -4921,7 +5109,7 @@
       </c>
       <c r="F2" s="28">
         <f>$B2+$C2+IF(($E2/$E$50&gt;$D2/$D$50),($E2/$E$50)*7.5, ($D2/$D$50)*3+($E2/$E$50)*4.5)</f>
-        <v>1.3955555555555554</v>
+        <v>1.3880555555555554</v>
       </c>
       <c r="G2" s="29">
         <f>0.5*INT(F2/0.5)+INT( ((F2-INT(F2/0.5)*0.5)/0.25))*0.5</f>
@@ -4942,7 +5130,7 @@
       </c>
       <c r="C3" s="28">
         <f>Homeworks!J3</f>
-        <v>1.2193749999999999</v>
+        <v>1.2716741071428572</v>
       </c>
       <c r="D3" s="26">
         <f>Exams!B3</f>
@@ -4954,7 +5142,7 @@
       </c>
       <c r="F3" s="28">
         <f t="shared" ref="F3:F48" si="0">$B3+$C3+IF(($E3/$E$50&gt;$D3/$D$50),($E3/$E$50)*7.5, ($D3/$D$50)*3+($E3/$E$50)*4.5)</f>
-        <v>4.1475231481481485</v>
+        <v>4.1998222552910054</v>
       </c>
       <c r="G3" s="29">
         <f t="shared" ref="G3:G48" si="1">0.5*INT(F3/0.5)+INT( ((F3-INT(F3/0.5)*0.5)/0.25))*0.5</f>
@@ -4975,7 +5163,7 @@
       </c>
       <c r="C4" s="28">
         <f>Homeworks!J4</f>
-        <v>1.39671875</v>
+        <v>1.4225390625000001</v>
       </c>
       <c r="D4" s="26">
         <f>Exams!B4</f>
@@ -4987,7 +5175,7 @@
       </c>
       <c r="F4" s="28">
         <f t="shared" si="0"/>
-        <v>4.4880150462962964</v>
+        <v>4.513835358796296</v>
       </c>
       <c r="G4" s="29">
         <f t="shared" si="1"/>
@@ -5008,7 +5196,7 @@
       </c>
       <c r="C5" s="28">
         <f>Homeworks!J5</f>
-        <v>0.20000000000000004</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="D5" s="26">
         <f>Exams!B5</f>
@@ -5020,7 +5208,7 @@
       </c>
       <c r="F5" s="28">
         <f t="shared" si="0"/>
-        <v>0.22222222222222227</v>
+        <v>0.17222222222222225</v>
       </c>
       <c r="G5" s="29">
         <f t="shared" si="1"/>
@@ -5041,7 +5229,7 @@
       </c>
       <c r="C6" s="28">
         <f>Homeworks!J6</f>
-        <v>0.45218749999999996</v>
+        <v>0.33914062499999997</v>
       </c>
       <c r="D6" s="26">
         <f>Exams!B6</f>
@@ -5053,7 +5241,7 @@
       </c>
       <c r="F6" s="28">
         <f t="shared" si="0"/>
-        <v>3.0349652777777774</v>
+        <v>2.921918402777778</v>
       </c>
       <c r="G6" s="29">
         <f t="shared" si="1"/>
@@ -5074,7 +5262,7 @@
       </c>
       <c r="C7" s="28">
         <f>Homeworks!J7</f>
-        <v>0.70874999999999988</v>
+        <v>0.86370535714285712</v>
       </c>
       <c r="D7" s="26">
         <f>Exams!B7</f>
@@ -5086,7 +5274,7 @@
       </c>
       <c r="F7" s="28">
         <f t="shared" si="0"/>
-        <v>2.3393055555555553</v>
+        <v>2.4942609126984125</v>
       </c>
       <c r="G7" s="29">
         <f t="shared" si="1"/>
@@ -5107,7 +5295,7 @@
       </c>
       <c r="C8" s="28">
         <f>Homeworks!J8</f>
-        <v>2.5000000000000005E-2</v>
+        <v>2.6785714285714284E-2</v>
       </c>
       <c r="D8" s="26">
         <f>Exams!B8</f>
@@ -5119,7 +5307,7 @@
       </c>
       <c r="F8" s="28">
         <f t="shared" si="0"/>
-        <v>1.0418518518518518</v>
+        <v>1.0436375661375661</v>
       </c>
       <c r="G8" s="29">
         <f t="shared" si="1"/>
@@ -5140,7 +5328,7 @@
       </c>
       <c r="C9" s="28">
         <f>Homeworks!J9</f>
-        <v>0.44968750000000002</v>
+        <v>0.39039062499999999</v>
       </c>
       <c r="D9" s="26">
         <f>Exams!B9</f>
@@ -5152,7 +5340,7 @@
       </c>
       <c r="F9" s="28">
         <f t="shared" si="0"/>
-        <v>2.3722800925925926</v>
+        <v>2.3129832175925928</v>
       </c>
       <c r="G9" s="29">
         <f t="shared" si="1"/>
@@ -5173,7 +5361,7 @@
       </c>
       <c r="C10" s="28">
         <f>Homeworks!J10</f>
-        <v>1.3321874999999999</v>
+        <v>1.3614174107142856</v>
       </c>
       <c r="D10" s="26">
         <f>Exams!B10</f>
@@ -5185,7 +5373,7 @@
       </c>
       <c r="F10" s="28">
         <f t="shared" si="0"/>
-        <v>3.7620023148148145</v>
+        <v>3.7912322255291002</v>
       </c>
       <c r="G10" s="29">
         <f t="shared" si="1"/>
@@ -5206,7 +5394,7 @@
       </c>
       <c r="C11" s="28">
         <f>Homeworks!J11</f>
-        <v>0.14250000000000002</v>
+        <v>0.10687500000000001</v>
       </c>
       <c r="D11" s="26">
         <f>Exams!B11</f>
@@ -5218,7 +5406,7 @@
       </c>
       <c r="F11" s="28">
         <f t="shared" si="0"/>
-        <v>2.2136111111111112</v>
+        <v>2.1779861111111112</v>
       </c>
       <c r="G11" s="29">
         <f t="shared" si="1"/>
@@ -5239,7 +5427,7 @@
       </c>
       <c r="C12" s="28">
         <f>Homeworks!J12</f>
-        <v>1.1681250000000001</v>
+        <v>1.0528794642857144</v>
       </c>
       <c r="D12" s="26">
         <f>Exams!B12</f>
@@ -5251,7 +5439,7 @@
       </c>
       <c r="F12" s="28">
         <f t="shared" si="0"/>
-        <v>3.398865740740741</v>
+        <v>3.2836202050264554</v>
       </c>
       <c r="G12" s="29">
         <f t="shared" si="1"/>
@@ -5272,7 +5460,7 @@
       </c>
       <c r="C13" s="28">
         <f>Homeworks!J13</f>
-        <v>0.94781250000000006</v>
+        <v>1.0313950892857142</v>
       </c>
       <c r="D13" s="26">
         <f>Exams!B13</f>
@@ -5284,7 +5472,7 @@
       </c>
       <c r="F13" s="28">
         <f t="shared" si="0"/>
-        <v>3.4613310185185187</v>
+        <v>3.5449136078042329</v>
       </c>
       <c r="G13" s="29">
         <f t="shared" si="1"/>
@@ -5305,7 +5493,7 @@
       </c>
       <c r="C14" s="28">
         <f>Homeworks!J14</f>
-        <v>0.52687500000000009</v>
+        <v>0.4889062500000001</v>
       </c>
       <c r="D14" s="26">
         <f>Exams!B14</f>
@@ -5317,7 +5505,7 @@
       </c>
       <c r="F14" s="28">
         <f t="shared" si="0"/>
-        <v>2.3213194444444447</v>
+        <v>2.2833506944444446</v>
       </c>
       <c r="G14" s="29">
         <f t="shared" si="1"/>
@@ -5338,7 +5526,7 @@
       </c>
       <c r="C15" s="28">
         <f>Homeworks!J15</f>
-        <v>0.66156250000000005</v>
+        <v>0.76112723214285716</v>
       </c>
       <c r="D15" s="26">
         <f>Exams!B15</f>
@@ -5350,7 +5538,7 @@
       </c>
       <c r="F15" s="28">
         <f t="shared" si="0"/>
-        <v>3.3489699074074073</v>
+        <v>3.4485346395502647</v>
       </c>
       <c r="G15" s="29">
         <f t="shared" si="1"/>
@@ -5371,7 +5559,7 @@
       </c>
       <c r="C16" s="28">
         <f>Homeworks!J16</f>
-        <v>1.2110937500000001</v>
+        <v>1.1868917410714286</v>
       </c>
       <c r="D16" s="26">
         <f>Exams!B16</f>
@@ -5383,7 +5571,7 @@
       </c>
       <c r="F16" s="28">
         <f t="shared" si="0"/>
-        <v>3.084797453703704</v>
+        <v>3.0605954447751325</v>
       </c>
       <c r="G16" s="29">
         <f t="shared" si="1"/>
@@ -5404,7 +5592,7 @@
       </c>
       <c r="C17" s="28">
         <f>Homeworks!J17</f>
-        <v>0.54812499999999997</v>
+        <v>0.72024553571428562</v>
       </c>
       <c r="D17" s="26">
         <f>Exams!B17</f>
@@ -5416,7 +5604,7 @@
       </c>
       <c r="F17" s="28">
         <f t="shared" si="0"/>
-        <v>2.2716435185185184</v>
+        <v>2.4437640542328039</v>
       </c>
       <c r="G17" s="29">
         <f t="shared" si="1"/>
@@ -5437,7 +5625,7 @@
       </c>
       <c r="C18" s="28">
         <f>Homeworks!J18</f>
-        <v>0.10843750000000001</v>
+        <v>8.1328125000000001E-2</v>
       </c>
       <c r="D18" s="26">
         <f>Exams!B18</f>
@@ -5449,7 +5637,7 @@
       </c>
       <c r="F18" s="28">
         <f t="shared" si="0"/>
-        <v>1.2919560185185186</v>
+        <v>1.2648466435185184</v>
       </c>
       <c r="G18" s="29">
         <f t="shared" si="1"/>
@@ -5470,7 +5658,7 @@
       </c>
       <c r="C19" s="28">
         <f>Homeworks!J19</f>
-        <v>1.09765625</v>
+        <v>1.1484654017857143</v>
       </c>
       <c r="D19" s="26">
         <f>Exams!B19</f>
@@ -5482,7 +5670,7 @@
       </c>
       <c r="F19" s="28">
         <f t="shared" si="0"/>
-        <v>3.0606192129629628</v>
+        <v>3.1114283647486776</v>
       </c>
       <c r="G19" s="29">
         <f t="shared" si="1"/>
@@ -5503,7 +5691,7 @@
       </c>
       <c r="C20" s="28">
         <f>Homeworks!J20</f>
-        <v>1.05078125</v>
+        <v>1.1282645089285714</v>
       </c>
       <c r="D20" s="26">
         <f>Exams!B20</f>
@@ -5515,7 +5703,7 @@
       </c>
       <c r="F20" s="28">
         <f t="shared" si="0"/>
-        <v>3.8383738425925928</v>
+        <v>3.9158571015211643</v>
       </c>
       <c r="G20" s="29">
         <f t="shared" si="1"/>
@@ -5536,7 +5724,7 @@
       </c>
       <c r="C21" s="28">
         <f>Homeworks!J21</f>
-        <v>0.93437500000000007</v>
+        <v>0.86685267857142878</v>
       </c>
       <c r="D21" s="26">
         <f>Exams!B21</f>
@@ -5548,7 +5736,7 @@
       </c>
       <c r="F21" s="28">
         <f t="shared" si="0"/>
-        <v>3.2484490740740739</v>
+        <v>3.1809267526455027</v>
       </c>
       <c r="G21" s="29">
         <f t="shared" si="1"/>
@@ -5569,7 +5757,7 @@
       </c>
       <c r="C22" s="28">
         <f>Homeworks!J22</f>
-        <v>1.3451562499999998</v>
+        <v>1.3758314732142858</v>
       </c>
       <c r="D22" s="26">
         <f>Exams!B22</f>
@@ -5581,7 +5769,7 @@
       </c>
       <c r="F22" s="28">
         <f t="shared" si="0"/>
-        <v>4.5244155092592591</v>
+        <v>4.5550907324735448</v>
       </c>
       <c r="G22" s="29">
         <f t="shared" si="1"/>
@@ -5602,7 +5790,7 @@
       </c>
       <c r="C23" s="28">
         <f>Homeworks!J23</f>
-        <v>1.0618750000000001</v>
+        <v>0.95171874999999995</v>
       </c>
       <c r="D23" s="26">
         <f>Exams!B23</f>
@@ -5614,7 +5802,7 @@
       </c>
       <c r="F23" s="28">
         <f t="shared" si="0"/>
-        <v>2.6707638888888892</v>
+        <v>2.560607638888889</v>
       </c>
       <c r="G23" s="29">
         <f t="shared" si="1"/>
@@ -5635,7 +5823,7 @@
       </c>
       <c r="C24" s="28">
         <f>Homeworks!J24</f>
-        <v>0.54937500000000006</v>
+        <v>0.61069196428571437</v>
       </c>
       <c r="D24" s="26">
         <f>Exams!B24</f>
@@ -5647,7 +5835,7 @@
       </c>
       <c r="F24" s="28">
         <f t="shared" si="0"/>
-        <v>3.0977083333333333</v>
+        <v>3.1590252976190474</v>
       </c>
       <c r="G24" s="29">
         <f t="shared" si="1"/>
@@ -5668,7 +5856,7 @@
       </c>
       <c r="C25" s="28">
         <f>Homeworks!J25</f>
-        <v>0.50593750000000004</v>
+        <v>0.59150669642857145</v>
       </c>
       <c r="D25" s="26">
         <f>Exams!B25</f>
@@ -5680,7 +5868,7 @@
       </c>
       <c r="F25" s="28">
         <f t="shared" si="0"/>
-        <v>2.3448263888888889</v>
+        <v>2.4303955853174606</v>
       </c>
       <c r="G25" s="29">
         <f t="shared" si="1"/>
@@ -5701,7 +5889,7 @@
       </c>
       <c r="C26" s="28">
         <f>Homeworks!J26</f>
-        <v>0.56812499999999999</v>
+        <v>0.74729910714285719</v>
       </c>
       <c r="D26" s="26">
         <f>Exams!B26</f>
@@ -5713,11 +5901,11 @@
       </c>
       <c r="F26" s="28">
         <f t="shared" si="0"/>
-        <v>2.1920138888888889</v>
+        <v>2.3711879960317459</v>
       </c>
       <c r="G26" s="29">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="H26" s="26">
         <f t="shared" si="2"/>
@@ -5734,7 +5922,7 @@
       </c>
       <c r="C27" s="28">
         <f>Homeworks!J27</f>
-        <v>0.54953125000000003</v>
+        <v>0.6050055803571428</v>
       </c>
       <c r="D27" s="26">
         <f>Exams!B27</f>
@@ -5746,7 +5934,7 @@
       </c>
       <c r="F27" s="28">
         <f t="shared" si="0"/>
-        <v>2.3154571759259257</v>
+        <v>2.3709315062830685</v>
       </c>
       <c r="G27" s="29">
         <f t="shared" si="1"/>
@@ -5767,7 +5955,7 @@
       </c>
       <c r="C28" s="28">
         <f>Homeworks!J28</f>
-        <v>8.8125000000000009E-2</v>
+        <v>0.11296875000000001</v>
       </c>
       <c r="D28" s="26">
         <f>Exams!B28</f>
@@ -5779,7 +5967,7 @@
       </c>
       <c r="F28" s="28">
         <f t="shared" si="0"/>
-        <v>1.6029398148148148</v>
+        <v>1.6277835648148149</v>
       </c>
       <c r="G28" s="29">
         <f t="shared" si="1"/>
@@ -5800,7 +5988,7 @@
       </c>
       <c r="C29" s="28">
         <f>Homeworks!J29</f>
-        <v>0.19499999999999998</v>
+        <v>0.28687499999999999</v>
       </c>
       <c r="D29" s="26">
         <f>Exams!B29</f>
@@ -5812,7 +6000,7 @@
       </c>
       <c r="F29" s="28">
         <f t="shared" si="0"/>
-        <v>1.4716666666666667</v>
+        <v>1.5635416666666666</v>
       </c>
       <c r="G29" s="29">
         <f t="shared" si="1"/>
@@ -5833,7 +6021,7 @@
       </c>
       <c r="C30" s="28">
         <f>Homeworks!J30</f>
-        <v>1.41</v>
+        <v>1.3907589285714286</v>
       </c>
       <c r="D30" s="26">
         <f>Exams!B30</f>
@@ -5845,7 +6033,7 @@
       </c>
       <c r="F30" s="28">
         <f t="shared" si="0"/>
-        <v>5.2181481481481491</v>
+        <v>5.1989070767195766</v>
       </c>
       <c r="G30" s="29">
         <f t="shared" si="1"/>
@@ -5866,7 +6054,7 @@
       </c>
       <c r="C31" s="28">
         <f>Homeworks!J31</f>
-        <v>0.75546875000000002</v>
+        <v>0.81861049107142869</v>
       </c>
       <c r="D31" s="26">
         <f>Exams!B31</f>
@@ -5878,7 +6066,7 @@
       </c>
       <c r="F31" s="28">
         <f t="shared" si="0"/>
-        <v>3.1336168981481483</v>
+        <v>3.1967586392195768</v>
       </c>
       <c r="G31" s="29">
         <f t="shared" si="1"/>
@@ -5899,7 +6087,7 @@
       </c>
       <c r="C32" s="28">
         <f>Homeworks!J32</f>
-        <v>0.82281249999999995</v>
+        <v>0.86755580357142847</v>
       </c>
       <c r="D32" s="26">
         <f>Exams!B32</f>
@@ -5911,7 +6099,7 @@
       </c>
       <c r="F32" s="28">
         <f t="shared" si="0"/>
-        <v>3.5952199074074076</v>
+        <v>3.639963210978836</v>
       </c>
       <c r="G32" s="29">
         <f t="shared" si="1"/>
@@ -5965,7 +6153,7 @@
       </c>
       <c r="C34" s="28">
         <f>Homeworks!J34</f>
-        <v>0.62375000000000003</v>
+        <v>0.67450892857142863</v>
       </c>
       <c r="D34" s="26">
         <f>Exams!B34</f>
@@ -5977,11 +6165,11 @@
       </c>
       <c r="F34" s="28">
         <f t="shared" si="0"/>
-        <v>3.2456018518518519</v>
+        <v>3.2963607804232802</v>
       </c>
       <c r="G34" s="29">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="H34" s="26">
         <f t="shared" si="2"/>
@@ -5998,7 +6186,7 @@
       </c>
       <c r="C35" s="28">
         <f>Homeworks!J35</f>
-        <v>0.19187499999999999</v>
+        <v>0.16801339285714284</v>
       </c>
       <c r="D35" s="26">
         <f>Exams!B35</f>
@@ -6010,7 +6198,7 @@
       </c>
       <c r="F35" s="28">
         <f t="shared" si="0"/>
-        <v>1.2383564814814814</v>
+        <v>1.2144948743386244</v>
       </c>
       <c r="G35" s="29">
         <f t="shared" si="1"/>
@@ -6097,7 +6285,7 @@
       </c>
       <c r="C38" s="28">
         <f>Homeworks!J38</f>
-        <v>0.55562500000000004</v>
+        <v>0.681450892857143</v>
       </c>
       <c r="D38" s="26">
         <f>Exams!B38</f>
@@ -6109,7 +6297,7 @@
       </c>
       <c r="F38" s="28">
         <f t="shared" si="0"/>
-        <v>2.3171064814814817</v>
+        <v>2.4429323743386249</v>
       </c>
       <c r="G38" s="29">
         <f t="shared" si="1"/>
@@ -6130,7 +6318,7 @@
       </c>
       <c r="C39" s="28">
         <f>Homeworks!J39</f>
-        <v>0.75749999999999995</v>
+        <v>0.65651785714285715</v>
       </c>
       <c r="D39" s="26">
         <f>Exams!B39</f>
@@ -6142,7 +6330,7 @@
       </c>
       <c r="F39" s="28">
         <f t="shared" si="0"/>
-        <v>3.1658333333333335</v>
+        <v>3.0648511904761904</v>
       </c>
       <c r="G39" s="29">
         <f t="shared" si="1"/>
@@ -6163,7 +6351,7 @@
       </c>
       <c r="C40" s="28">
         <f>Homeworks!J40</f>
-        <v>0.22437499999999999</v>
+        <v>0.38569196428571428</v>
       </c>
       <c r="D40" s="26">
         <f>Exams!B40</f>
@@ -6175,7 +6363,7 @@
       </c>
       <c r="F40" s="28">
         <f t="shared" si="0"/>
-        <v>1.8171527777777778</v>
+        <v>1.978469742063492</v>
       </c>
       <c r="G40" s="29">
         <f t="shared" si="1"/>
@@ -6196,7 +6384,7 @@
       </c>
       <c r="C41" s="28">
         <f>Homeworks!J41</f>
-        <v>1.34078125</v>
+        <v>1.3645145089285715</v>
       </c>
       <c r="D41" s="26">
         <f>Exams!B41</f>
@@ -6208,7 +6396,7 @@
       </c>
       <c r="F41" s="28">
         <f t="shared" si="0"/>
-        <v>4.4352256944444441</v>
+        <v>4.4589589533730161</v>
       </c>
       <c r="G41" s="29">
         <f t="shared" si="1"/>
@@ -6229,7 +6417,7 @@
       </c>
       <c r="C42" s="28">
         <f>Homeworks!J42</f>
-        <v>0.26375000000000004</v>
+        <v>0.48040178571428571</v>
       </c>
       <c r="D42" s="26">
         <f>Exams!B42</f>
@@ -6241,11 +6429,11 @@
       </c>
       <c r="F42" s="28">
         <f t="shared" si="0"/>
-        <v>1.240601851851852</v>
+        <v>1.4572536375661378</v>
       </c>
       <c r="G42" s="29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H42" s="26">
         <f t="shared" si="2"/>
@@ -6262,7 +6450,7 @@
       </c>
       <c r="C43" s="28">
         <f>Homeworks!J43</f>
-        <v>1.1612500000000001</v>
+        <v>1.2162500000000001</v>
       </c>
       <c r="D43" s="26">
         <f>Exams!B43</f>
@@ -6274,7 +6462,7 @@
       </c>
       <c r="F43" s="28">
         <f t="shared" si="0"/>
-        <v>4.4534722222222225</v>
+        <v>4.5084722222222222</v>
       </c>
       <c r="G43" s="29">
         <f t="shared" si="1"/>
@@ -6295,7 +6483,7 @@
       </c>
       <c r="C44" s="28">
         <f>Homeworks!J44</f>
-        <v>0.92937499999999995</v>
+        <v>1.0418973214285714</v>
       </c>
       <c r="D44" s="26">
         <f>Exams!B44</f>
@@ -6307,7 +6495,7 @@
       </c>
       <c r="F44" s="28">
         <f t="shared" si="0"/>
-        <v>2.9619675925925923</v>
+        <v>3.0744899140211639</v>
       </c>
       <c r="G44" s="29">
         <f t="shared" si="1"/>
@@ -6361,7 +6549,7 @@
       </c>
       <c r="C46" s="28">
         <f>Homeworks!J46</f>
-        <v>0.81859375000000012</v>
+        <v>0.89073102678571425</v>
       </c>
       <c r="D46" s="26">
         <f>Exams!B46</f>
@@ -6373,7 +6561,7 @@
       </c>
       <c r="F46" s="28">
         <f t="shared" si="0"/>
-        <v>2.5854456018518519</v>
+        <v>2.6575828786375659</v>
       </c>
       <c r="G46" s="29">
         <f t="shared" si="1"/>
@@ -6394,7 +6582,7 @@
       </c>
       <c r="C47" s="28">
         <f>Homeworks!J47</f>
-        <v>0.34703124999999996</v>
+        <v>0.26027343749999998</v>
       </c>
       <c r="D47" s="26">
         <f>Exams!B47</f>
@@ -6406,7 +6594,7 @@
       </c>
       <c r="F47" s="28">
         <f t="shared" si="0"/>
-        <v>2.2240682870370367</v>
+        <v>2.137310474537037</v>
       </c>
       <c r="G47" s="29">
         <f t="shared" si="1"/>
@@ -6427,7 +6615,7 @@
       </c>
       <c r="C48" s="28">
         <f>Homeworks!J48</f>
-        <v>0.21406249999999996</v>
+        <v>0.16054687499999998</v>
       </c>
       <c r="D48" s="26">
         <f>Exams!B48</f>
@@ -6439,7 +6627,7 @@
       </c>
       <c r="F48" s="28">
         <f t="shared" si="0"/>
-        <v>0.66869212962962954</v>
+        <v>0.61517650462962958</v>
       </c>
       <c r="G48" s="29">
         <f t="shared" si="1"/>
@@ -6492,7 +6680,7 @@
       </c>
       <c r="C51" s="13">
         <f t="shared" ref="C51:H51" si="5">AVERAGE(C$2:C$48)</f>
-        <v>0.62746010638297889</v>
+        <v>0.65448945668693015</v>
       </c>
       <c r="D51" s="13">
         <f t="shared" si="5"/>
@@ -6504,11 +6692,11 @@
       </c>
       <c r="F51" s="13">
         <f t="shared" si="5"/>
-        <v>2.4947532505910166</v>
+        <v>2.521782600894968</v>
       </c>
       <c r="G51" s="13">
         <f t="shared" si="5"/>
-        <v>2.478723404255319</v>
+        <v>2.5106382978723403</v>
       </c>
       <c r="H51" s="13">
         <f t="shared" si="5"/>
@@ -6525,7 +6713,7 @@
       </c>
       <c r="C52" s="13">
         <f t="shared" ref="C52:H52" si="6">STDEV(C$2:C$48)</f>
-        <v>0.44949257777572238</v>
+        <v>0.45797216731590284</v>
       </c>
       <c r="D52" s="13">
         <f t="shared" si="6"/>
@@ -6537,11 +6725,11 @@
       </c>
       <c r="F52" s="13">
         <f t="shared" si="6"/>
-        <v>1.30873837630002</v>
+        <v>1.3147149100958579</v>
       </c>
       <c r="G52" s="13">
         <f t="shared" si="6"/>
-        <v>1.3185855679827938</v>
+        <v>1.3125206487076675</v>
       </c>
       <c r="H52" s="13">
         <f t="shared" si="6"/>
@@ -6558,7 +6746,7 @@
       </c>
       <c r="C53" s="13">
         <f t="shared" ref="C53:H53" si="7">MEDIAN(C$2:C$48)</f>
-        <v>0.55562500000000004</v>
+        <v>0.67450892857142863</v>
       </c>
       <c r="D53" s="13">
         <f t="shared" si="7"/>
@@ -6570,7 +6758,7 @@
       </c>
       <c r="F53" s="13">
         <f t="shared" si="7"/>
-        <v>2.3722800925925926</v>
+        <v>2.4942609126984125</v>
       </c>
       <c r="G53" s="13">
         <f t="shared" si="7"/>

</xml_diff>